<commit_message>
LESSON16 - SQLD1 - 16.03.2024
</commit_message>
<xml_diff>
--- a/java21 database design/Java21 QPhan Database Design.xlsx
+++ b/java21 database design/Java21 QPhan Database Design.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java21\3. Database\java21 database design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F8F162-F57D-4143-BD49-45036BC35D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E15D668-C3A7-440B-8091-C62DEA68CFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
     <sheet name="B2. Mô hình logic" sheetId="2" r:id="rId2"/>
     <sheet name="B3. Mô hình vật lý" sheetId="4" r:id="rId3"/>
+    <sheet name="Bn. Tạo dữ liệu kiểm thử" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -174,6 +175,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={8EC58335-C900-492B-BA28-EE6A8C506FC5}</author>
+    <author>Quyen Ngoc Phan</author>
     <author>tc={34745E4D-1BCF-46E0-8BDB-A445EE5E1BD2}</author>
     <author>tc={C1921E78-7869-444A-8472-B8D666CCBAC5}</author>
     <author>tc={1305DD5C-A913-487C-8B38-59BD0DFB2D0F}</author>
@@ -195,7 +197,32 @@
     Không cần thuộc phòng ban, làm được mọi chức năng</t>
       </text>
     </comment>
-    <comment ref="E6" authorId="1" shapeId="0" xr:uid="{34745E4D-1BCF-46E0-8BDB-A445EE5E1BD2}">
+    <comment ref="K4" authorId="1" shapeId="0" xr:uid="{B746EB97-6D3C-4F53-97FC-412D4E572F20}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Bảng doanh thu, lưu doanh thu bán hàng từ ngày from đến ngày until số tiền bao nhiêu
+Chưa xử lý lưu trữ danh sách mặt hàng, đơn hàng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="2" shapeId="0" xr:uid="{34745E4D-1BCF-46E0-8BDB-A445EE5E1BD2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -203,7 +230,7 @@
     Tiền mặt, thẻ tín dụng, thẻ ghi nợ, ví điện tử</t>
       </text>
     </comment>
-    <comment ref="F6" authorId="2" shapeId="0" xr:uid="{C1921E78-7869-444A-8472-B8D666CCBAC5}">
+    <comment ref="F6" authorId="3" shapeId="0" xr:uid="{C1921E78-7869-444A-8472-B8D666CCBAC5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -211,7 +238,32 @@
     Chờ xác nhận, Đang đóng gói, Đóng gói hoàn thành chờ vận chuyển, Đang vận chuyển, Giao hàng thành công, Giao hàng thất bại, Hủy đơn hàng</t>
       </text>
     </comment>
-    <comment ref="B7" authorId="3" shapeId="0" xr:uid="{1305DD5C-A913-487C-8B38-59BD0DFB2D0F}">
+    <comment ref="J6" authorId="1" shapeId="0" xr:uid="{BFDAA607-05E3-4FA6-9169-4193A867187B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Lưu KDL DATE
+VD: 25/03 --&gt; tương ứng với ngày 25/03 0H0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="4" shapeId="0" xr:uid="{1305DD5C-A913-487C-8B38-59BD0DFB2D0F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -219,7 +271,33 @@
     Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</t>
       </text>
     </comment>
-    <comment ref="J8" authorId="4" shapeId="0" xr:uid="{F01BC811-4E6C-4543-AA25-E955BE8491CD}">
+    <comment ref="J7" authorId="1" shapeId="0" xr:uid="{464FAC46-B928-4D1B-B9FC-CA444F74AF8B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Lưu KDL DATE
+VD: 28/03 --&gt; tương ứng với ngày 28/3 23H59H59
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="5" shapeId="0" xr:uid="{F01BC811-4E6C-4543-AA25-E955BE8491CD}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -228,7 +306,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="M8" authorId="5" shapeId="0" xr:uid="{3702AC3F-ACCB-4FA5-81F8-3D4343E0ECEF}">
+    <comment ref="M8" authorId="6" shapeId="0" xr:uid="{3702AC3F-ACCB-4FA5-81F8-3D4343E0ECEF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -236,7 +314,7 @@
     Có rất nhiều màu sắc color, rgb, hexa -&gt; sử dụng varchar để lưu chứ k tạo 1 bảng riêng</t>
       </text>
     </comment>
-    <comment ref="J9" authorId="6" shapeId="0" xr:uid="{9527FEF5-CCFC-4F64-97A2-BBE2E29C2803}">
+    <comment ref="J9" authorId="7" shapeId="0" xr:uid="{9527FEF5-CCFC-4F64-97A2-BBE2E29C2803}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -244,7 +322,7 @@
     How - tính số lượng tồn kho theo giai đoạn ?</t>
       </text>
     </comment>
-    <comment ref="K9" authorId="7" shapeId="0" xr:uid="{3DE62A8D-5F5B-409E-A562-B1F200B29412}">
+    <comment ref="K9" authorId="8" shapeId="0" xr:uid="{3DE62A8D-5F5B-409E-A562-B1F200B29412}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -252,7 +330,7 @@
     Lưu thông tin bán những mặt hàng nào số lượng bao nhiêu, JSON, OBJECT</t>
       </text>
     </comment>
-    <comment ref="J10" authorId="8" shapeId="0" xr:uid="{43CCAF04-133F-49FE-87EB-557285BF8E90}">
+    <comment ref="J10" authorId="9" shapeId="0" xr:uid="{43CCAF04-133F-49FE-87EB-557285BF8E90}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -260,7 +338,7 @@
     Doanh thu cho mặt hàng theo giai đoạn</t>
       </text>
     </comment>
-    <comment ref="M10" authorId="9" shapeId="0" xr:uid="{2853FC81-A62F-4574-A1AA-7A29E9B44A89}">
+    <comment ref="M10" authorId="10" shapeId="0" xr:uid="{2853FC81-A62F-4574-A1AA-7A29E9B44A89}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -268,7 +346,7 @@
     Số lượng hàng còn lại ở thời điểm hiện tại</t>
       </text>
     </comment>
-    <comment ref="H12" authorId="10" shapeId="0" xr:uid="{B9E52DF8-6EBC-4DCF-8C8A-1994D6E5BB03}">
+    <comment ref="H12" authorId="11" shapeId="0" xr:uid="{B9E52DF8-6EBC-4DCF-8C8A-1994D6E5BB03}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -276,7 +354,7 @@
     NhanVien, Quan Ly</t>
       </text>
     </comment>
-    <comment ref="I22" authorId="11" shapeId="0" xr:uid="{4B47AF2D-C770-4A5E-8158-147A119469B1}">
+    <comment ref="I22" authorId="12" shapeId="0" xr:uid="{4B47AF2D-C770-4A5E-8158-147A119469B1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -288,8 +366,176 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={3503BA87-F97B-4BA2-B285-74026B5E7BB4}</author>
+    <author>tc={F417F53F-78F4-4FB2-9932-6B06E3741ADD}</author>
+    <author>tc={73A9844D-439C-4A34-96F0-71631781CCF8}</author>
+    <author>tc={89D0F75C-16FA-43DB-9BE0-099B1CAFC699}</author>
+    <author>tc={81011C5D-5AE3-44B3-97CD-014DF419A278}</author>
+    <author>Quyen Ngoc Phan</author>
+    <author>tc={D45AF084-4675-422C-9958-D87148145BEA}</author>
+    <author>tc={BFF9823B-C3B1-4818-99DA-2E82CF873073}</author>
+    <author>tc={AE19BEC5-BB6C-4F20-A9C5-16CD0C497F85}</author>
+    <author>tc={686C344B-1B7B-4A75-97B6-A6A7B29739FE}</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{3503BA87-F97B-4BA2-B285-74026B5E7BB4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</t>
+      </text>
+    </comment>
+    <comment ref="K5" authorId="1" shapeId="0" xr:uid="{F417F53F-78F4-4FB2-9932-6B06E3741ADD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Chờ xác nhận, Đang đóng gói, Đóng gói hoàn thành chờ vận chuyển, Đang vận chuyển, Giao hàng thành công, Giao hàng thất bại, Hủy đơn hàng</t>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="2" shapeId="0" xr:uid="{73A9844D-439C-4A34-96F0-71631781CCF8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Tiền mặt, thẻ tín dụng, thẻ ghi nợ, ví điện tử</t>
+      </text>
+    </comment>
+    <comment ref="B56" authorId="3" shapeId="0" xr:uid="{89D0F75C-16FA-43DB-9BE0-099B1CAFC699}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Không cần thuộc phòng ban, làm được mọi chức năng</t>
+      </text>
+    </comment>
+    <comment ref="I57" authorId="4" shapeId="0" xr:uid="{81011C5D-5AE3-44B3-97CD-014DF419A278}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NhanVien, Quan Ly</t>
+      </text>
+    </comment>
+    <comment ref="C71" authorId="5" shapeId="0" xr:uid="{97B38917-3C27-42E5-A452-A7A63273C962}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Lưu KDL DATE
+VD: 25/03 --&gt; tương ứng với ngày 25/03 0H0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D71" authorId="5" shapeId="0" xr:uid="{89BC852F-A852-42D9-8A07-73738E7D49A8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Lưu KDL DATE
+VD: 28/03 --&gt; tương ứng với ngày 28/3 23H59H59
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E71" authorId="6" shapeId="0" xr:uid="{D45AF084-4675-422C-9958-D87148145BEA}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Số lượng bán
+</t>
+      </text>
+    </comment>
+    <comment ref="F71" authorId="7" shapeId="0" xr:uid="{BFF9823B-C3B1-4818-99DA-2E82CF873073}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Doanh thu cho mặt hàng theo giai đoạn</t>
+      </text>
+    </comment>
+    <comment ref="B76" authorId="5" shapeId="0" xr:uid="{3308BC73-AD5E-408B-A255-F1435759065A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Bảng doanh thu, lưu doanh thu bán hàng từ ngày from đến ngày until số tiền bao nhiêu
+Chưa xử lý lưu trữ danh sách mặt hàng, đơn hàng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E84" authorId="8" shapeId="0" xr:uid="{AE19BEC5-BB6C-4F20-A9C5-16CD0C497F85}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Có rất nhiều màu sắc color, rgb, hexa -&gt; sử dụng varchar để lưu chứ k tạo 1 bảng riêng</t>
+      </text>
+    </comment>
+    <comment ref="G84" authorId="9" shapeId="0" xr:uid="{686C344B-1B7B-4A75-97B6-A6A7B29739FE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Số lượng hàng còn lại ở thời điểm hiện tại</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="369">
   <si>
     <t>NhanVien</t>
   </si>
@@ -976,18 +1222,6 @@
     <t>C11_CUSTOMER_EMAIL</t>
   </si>
   <si>
-    <t>C11_EMPLOYEE_ADDRESS</t>
-  </si>
-  <si>
-    <t>C11_EMPLOYEE_PHONE</t>
-  </si>
-  <si>
-    <t>C11_EMPLOYEE_USERNAME</t>
-  </si>
-  <si>
-    <t>C11_EMPLOYEE_PASSWORD</t>
-  </si>
-  <si>
     <t>Mô hình logic trên cơ sở đối tượng ==&gt; https://app.diagrams.net/#G1EC3kWNgwWJ-jrYKf-W24OTGjAV-pxvRf#%7B%22pageId%22%3A%22AbEYu_0bn73_d0lKOqK0%22%7D</t>
   </si>
   <si>
@@ -1001,13 +1235,451 @@
   </si>
   <si>
     <t>C09_DATE_UNTIL 23:59:59</t>
+  </si>
+  <si>
+    <t>C11_CUSTOMER_ADDRESS</t>
+  </si>
+  <si>
+    <t>C11_CUSTOMER_PHONE</t>
+  </si>
+  <si>
+    <t>C11_CUSTOMER_USERNAME</t>
+  </si>
+  <si>
+    <t>C11_CUSTOMER_PASSWORD</t>
+  </si>
+  <si>
+    <t>C15_LAST_UPDATED</t>
+  </si>
+  <si>
+    <t>[from, until]</t>
+  </si>
+  <si>
+    <t>Áo</t>
+  </si>
+  <si>
+    <t>Quần</t>
+  </si>
+  <si>
+    <t>Giày</t>
+  </si>
+  <si>
+    <t>Dép</t>
+  </si>
+  <si>
+    <t>Mũ</t>
+  </si>
+  <si>
+    <t>Thắt lưng</t>
+  </si>
+  <si>
+    <t>Túi xách</t>
+  </si>
+  <si>
+    <t>Áo 1</t>
+  </si>
+  <si>
+    <t>Áo 2</t>
+  </si>
+  <si>
+    <t>Áo 3</t>
+  </si>
+  <si>
+    <t>Quần 4</t>
+  </si>
+  <si>
+    <t>Quần 5</t>
+  </si>
+  <si>
+    <t>Giày 6</t>
+  </si>
+  <si>
+    <t>Giày 7</t>
+  </si>
+  <si>
+    <t>Giày 8</t>
+  </si>
+  <si>
+    <t>Giày 9</t>
+  </si>
+  <si>
+    <t>Giày 10</t>
+  </si>
+  <si>
+    <t>Giép 11</t>
+  </si>
+  <si>
+    <t>Áo 12</t>
+  </si>
+  <si>
+    <t>Giép 13</t>
+  </si>
+  <si>
+    <t>Mũ 14</t>
+  </si>
+  <si>
+    <t>Mũ 15</t>
+  </si>
+  <si>
+    <t>Thắt lưng 16</t>
+  </si>
+  <si>
+    <t>Thắt lưng 17</t>
+  </si>
+  <si>
+    <t>Mũ 18</t>
+  </si>
+  <si>
+    <t>Túi xách 1</t>
+  </si>
+  <si>
+    <t>Túi xách 2</t>
+  </si>
+  <si>
+    <t>Tiền mặt</t>
+  </si>
+  <si>
+    <t>Thẻ tín dụng</t>
+  </si>
+  <si>
+    <t>Thẻ ghi nợ</t>
+  </si>
+  <si>
+    <t>Ví điện tử</t>
+  </si>
+  <si>
+    <t>c1@gmal.com</t>
+  </si>
+  <si>
+    <t>c2@gmal.com</t>
+  </si>
+  <si>
+    <t>c3@gmal.com</t>
+  </si>
+  <si>
+    <t>c4@gmal.com</t>
+  </si>
+  <si>
+    <t>c5@gmal.com</t>
+  </si>
+  <si>
+    <t>c6@gmal.com</t>
+  </si>
+  <si>
+    <t>c7@gmal.com</t>
+  </si>
+  <si>
+    <t>c8@gmal.com</t>
+  </si>
+  <si>
+    <t>c9@gmal.com</t>
+  </si>
+  <si>
+    <t>c10@gmal.com</t>
+  </si>
+  <si>
+    <t>Lê Tèo</t>
+  </si>
+  <si>
+    <t>Văn An</t>
+  </si>
+  <si>
+    <t>Nguyễn A</t>
+  </si>
+  <si>
+    <t>Phan Tuấn</t>
+  </si>
+  <si>
+    <t>Hoàng Tiên</t>
+  </si>
+  <si>
+    <t>Phạm Ngọc</t>
+  </si>
+  <si>
+    <t>Đoạn Tú</t>
+  </si>
+  <si>
+    <t>Hoàng B</t>
+  </si>
+  <si>
+    <t>Lê Huân</t>
+  </si>
+  <si>
+    <t>Nam Ban</t>
+  </si>
+  <si>
+    <t>Địa chỉ 1</t>
+  </si>
+  <si>
+    <t>Địa chỉ 2</t>
+  </si>
+  <si>
+    <t>Địa chỉ 3</t>
+  </si>
+  <si>
+    <t>Địa chỉ 4</t>
+  </si>
+  <si>
+    <t>Địa chỉ 5</t>
+  </si>
+  <si>
+    <t>Địa chỉ 6</t>
+  </si>
+  <si>
+    <t>Địa chỉ 7</t>
+  </si>
+  <si>
+    <t>Địa chỉ 8</t>
+  </si>
+  <si>
+    <t>Địa chỉ 9</t>
+  </si>
+  <si>
+    <t>Địa chỉ 10</t>
+  </si>
+  <si>
+    <t>c1def</t>
+  </si>
+  <si>
+    <t>c3def</t>
+  </si>
+  <si>
+    <t>c5def</t>
+  </si>
+  <si>
+    <t>c7def</t>
+  </si>
+  <si>
+    <t>c9def</t>
+  </si>
+  <si>
+    <t>c2auto</t>
+  </si>
+  <si>
+    <t>c4auto</t>
+  </si>
+  <si>
+    <t>c6auto</t>
+  </si>
+  <si>
+    <t>c8auto</t>
+  </si>
+  <si>
+    <t>c10auto</t>
+  </si>
+  <si>
+    <t>$2a$12$w0bs0MW/O3nTyMhuv0r1jOjq2gOaxLxkZgms7u/khHRmtCh3S/Hpu</t>
+  </si>
+  <si>
+    <t>10.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>12.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>14.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>16.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>18.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>20.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>26.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>28.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>Địa chỉ 11</t>
+  </si>
+  <si>
+    <t>Địa chỉ 12</t>
+  </si>
+  <si>
+    <t>Địa chỉ 13</t>
+  </si>
+  <si>
+    <t>Dùng công thức để tính</t>
+  </si>
+  <si>
+    <t>Chờ xác nhận</t>
+  </si>
+  <si>
+    <t>Đang đóng gói</t>
+  </si>
+  <si>
+    <t>Đóng gói hoàn thành</t>
+  </si>
+  <si>
+    <t>Đang vận chuyển</t>
+  </si>
+  <si>
+    <t>Giao hàng thành công</t>
+  </si>
+  <si>
+    <t>Giao hàng thất bại</t>
+  </si>
+  <si>
+    <t>Hủy đơn hàng</t>
+  </si>
+  <si>
+    <t>Size 'S' cho Nữ</t>
+  </si>
+  <si>
+    <t>Size 'M' cho Nữ</t>
+  </si>
+  <si>
+    <t>Size 'L' cho Nữ</t>
+  </si>
+  <si>
+    <t>Size 'XL' cho Nữ</t>
+  </si>
+  <si>
+    <t>Size 'XXL' cho Nữ</t>
+  </si>
+  <si>
+    <t>Size 'S' cho Nam</t>
+  </si>
+  <si>
+    <t>Size 'M' cho Nam</t>
+  </si>
+  <si>
+    <t>Size 'L' cho Nam</t>
+  </si>
+  <si>
+    <t>Size 'XL' cho Nam</t>
+  </si>
+  <si>
+    <t>Size 'XXL' cho Nam</t>
+  </si>
+  <si>
+    <t>Nhân viên</t>
+  </si>
+  <si>
+    <t>Trưởng bộ phận</t>
+  </si>
+  <si>
+    <t>Chủ sở hữu</t>
+  </si>
+  <si>
+    <t>Giảm đốc</t>
+  </si>
+  <si>
+    <t>Nhân viên 1</t>
+  </si>
+  <si>
+    <t>Nhân viên 2</t>
+  </si>
+  <si>
+    <t>Nhân viên 4</t>
+  </si>
+  <si>
+    <t>Nhân viên 3</t>
+  </si>
+  <si>
+    <t>Nhân viên 5</t>
+  </si>
+  <si>
+    <t>Nhân viên 6</t>
+  </si>
+  <si>
+    <t>Nhân viên 7</t>
+  </si>
+  <si>
+    <t>Nhân viên 8</t>
+  </si>
+  <si>
+    <t>Nhân viên 9</t>
+  </si>
+  <si>
+    <t>Nhân viên 10</t>
+  </si>
+  <si>
+    <t>nv1@gmal.com</t>
+  </si>
+  <si>
+    <t>nv2@gmal.com</t>
+  </si>
+  <si>
+    <t>nv1def</t>
+  </si>
+  <si>
+    <t>nv2auto</t>
+  </si>
+  <si>
+    <t>nv3def</t>
+  </si>
+  <si>
+    <t>nv4auto</t>
+  </si>
+  <si>
+    <t>nv5def</t>
+  </si>
+  <si>
+    <t>nv6auto</t>
+  </si>
+  <si>
+    <t>nv7def</t>
+  </si>
+  <si>
+    <t>nv8auto</t>
+  </si>
+  <si>
+    <t>nv9def</t>
+  </si>
+  <si>
+    <t>nv10auto</t>
+  </si>
+  <si>
+    <t>C09_DATE_FROM</t>
+  </si>
+  <si>
+    <t>C09_DATE_UNTIL</t>
+  </si>
+  <si>
+    <t>Bài tập phần DML - Tạo câu truy vấn để xử lý</t>
+  </si>
+  <si>
+    <t>C10_DATE_FROM</t>
+  </si>
+  <si>
+    <t>C10_DATE_UNITIL</t>
+  </si>
+  <si>
+    <t>Sử dụng dữ liệu từ các bảng ITEM, SIZE
+---
+ITEM, SIZE có ID lẻ: AMOUNT = 125, SALES_PRICE = BUY_PRICE * 2 + SIZE_ID * 5
+ITEM, SIZE có ID lẻ: AMOUNT = 280, SALES_PRICE = BUY_PRICE * 2 + SIZE_ID * 5 + 20</t>
+  </si>
+  <si>
+    <t>Sử dụng ITEM ID từ bảng ITEM và fake default path</t>
+  </si>
+  <si>
+    <t>Large amount of data</t>
+  </si>
+  <si>
+    <t>-- 1. Đơn hàng từ 1 - 5 --&gt; Giao thành công (trạng thái từ 1 - 6)</t>
+  </si>
+  <si>
+    <t>-- 2 Đơn hàng từ 6 - 8 --&gt; Đóng gói thành công (trạng thái từ 1 - 4)</t>
+  </si>
+  <si>
+    <t>-- 3. Đơn hàng từ 9 - 10 --&gt; Đang giao hàng (trạng thái từ 1 - 5)</t>
+  </si>
+  <si>
+    <t>-- 4. Đơn hàng từ 11 - 12 --&gt; Hủy đơn hàng (trạng thái 7)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1129,10 +1801,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="12"/>
-      <color rgb="FFC00000"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1142,6 +1838,14 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1164,7 +1868,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1200,11 +1904,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1290,9 +2004,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1301,6 +2012,21 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1314,8 +2040,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1692,6 +2437,39 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D4" dT="2024-03-19T12:47:34.71" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{3503BA87-F97B-4BA2-B285-74026B5E7BB4}">
+    <text>Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</text>
+  </threadedComment>
+  <threadedComment ref="K5" dT="2024-04-06T14:25:21.49" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{F417F53F-78F4-4FB2-9932-6B06E3741ADD}">
+    <text>Chờ xác nhận, Đang đóng gói, Đóng gói hoàn thành chờ vận chuyển, Đang vận chuyển, Giao hàng thành công, Giao hàng thất bại, Hủy đơn hàng</text>
+  </threadedComment>
+  <threadedComment ref="H15" dT="2024-04-06T14:23:17.00" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{73A9844D-439C-4A34-96F0-71631781CCF8}">
+    <text>Tiền mặt, thẻ tín dụng, thẻ ghi nợ, ví điện tử</text>
+  </threadedComment>
+  <threadedComment ref="B56" dT="2024-03-19T13:48:38.72" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{89D0F75C-16FA-43DB-9BE0-099B1CAFC699}">
+    <text>Không cần thuộc phòng ban, làm được mọi chức năng</text>
+  </threadedComment>
+  <threadedComment ref="I57" dT="2024-03-19T13:49:56.69" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{81011C5D-5AE3-44B3-97CD-014DF419A278}">
+    <text>NhanVien, Quan Ly</text>
+  </threadedComment>
+  <threadedComment ref="E71" dT="2024-04-02T13:49:52.63" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{D45AF084-4675-422C-9958-D87148145BEA}">
+    <text xml:space="preserve">Số lượng bán
+</text>
+  </threadedComment>
+  <threadedComment ref="F71" dT="2024-04-02T13:55:15.51" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{BFF9823B-C3B1-4818-99DA-2E82CF873073}">
+    <text>Doanh thu cho mặt hàng theo giai đoạn</text>
+  </threadedComment>
+  <threadedComment ref="E84" dT="2024-04-02T12:50:53.71" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{AE19BEC5-BB6C-4F20-A9C5-16CD0C497F85}">
+    <text>Có rất nhiều màu sắc color, rgb, hexa -&gt; sử dụng varchar để lưu chứ k tạo 1 bảng riêng</text>
+  </threadedComment>
+  <threadedComment ref="G84" dT="2024-04-02T13:53:18.17" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{686C344B-1B7B-4A75-97B6-A6A7B29739FE}">
+    <text>Số lượng hàng còn lại ở thời điểm hiện tại</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L35"/>
@@ -2113,7 +2891,7 @@
   <dimension ref="B1:L35"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2133,12 +2911,12 @@
   <sheetData>
     <row r="1" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2754,8 +3532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258E744B-65C2-4DE9-994B-E5E54772E544}">
   <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4:P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2782,12 +3560,12 @@
   <sheetData>
     <row r="1" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="2" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2803,7 +3581,9 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="J3" s="6" t="s">
+        <v>229</v>
+      </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
@@ -2879,16 +3659,16 @@
       <c r="I5" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="J5" s="29" t="s">
+      <c r="J5" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="15" t="s">
         <v>211</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="31" t="s">
         <v>168</v>
       </c>
       <c r="N5" s="15" t="s">
@@ -2926,13 +3706,13 @@
       <c r="I6" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="J6" s="32" t="s">
         <v>210</v>
       </c>
       <c r="K6" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="3" t="s">
         <v>217</v>
       </c>
       <c r="M6" s="20" t="s">
@@ -2941,7 +3721,7 @@
       <c r="N6" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="O6" s="31" t="s">
         <v>170</v>
       </c>
       <c r="P6" s="15" t="s">
@@ -2965,8 +3745,8 @@
         <v>194</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="15" t="s">
-        <v>227</v>
+      <c r="J7" s="32" t="s">
+        <v>223</v>
       </c>
       <c r="K7" s="15" t="s">
         <v>214</v>
@@ -3009,7 +3789,7 @@
         <v>213</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="M8" s="20" t="s">
         <v>144</v>
@@ -3017,7 +3797,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3" t="s">
-        <v>176</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -3036,11 +3816,11 @@
       <c r="J9" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="31" t="s">
+      <c r="K9" s="30" t="s">
         <v>215</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>142</v>
@@ -3065,9 +3845,9 @@
       <c r="J10" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="3" t="s">
-        <v>221</v>
+      <c r="K10" s="30"/>
+      <c r="L10" s="20" t="s">
+        <v>226</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>148</v>
@@ -3092,7 +3872,7 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
@@ -3111,7 +3891,7 @@
       <c r="H12" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="I12" s="30"/>
+      <c r="I12" s="29"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -3127,9 +3907,8 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="30"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -3156,7 +3935,7 @@
     </row>
     <row r="15" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
-      <c r="C15" s="30"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -3165,7 +3944,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="30"/>
+      <c r="L15" s="29"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
@@ -3174,7 +3953,7 @@
     <row r="16" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="30"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -3235,20 +4014,20 @@
       </c>
     </row>
     <row r="21" spans="2:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
       <c r="K21" s="1" t="s">
         <v>208</v>
       </c>
@@ -3280,12 +4059,12 @@
       </c>
     </row>
     <row r="23" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
       <c r="F23" s="1">
         <v>1</v>
       </c>
@@ -3329,12 +4108,12 @@
       </c>
     </row>
     <row r="25" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
       <c r="F25" s="1">
         <v>3</v>
       </c>
@@ -3378,22 +4157,22 @@
       </c>
     </row>
     <row r="27" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="33" t="s">
+      <c r="B27" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="33"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="33" t="s">
+      <c r="B28" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="1" t="s">
         <v>173</v>
       </c>
@@ -3401,12 +4180,12 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="2:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="17" t="s">
         <v>174</v>
       </c>
@@ -3638,4 +4417,1923 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8B0AB7-EB07-4BA0-B0D1-595B07C9234C}">
+  <dimension ref="B1:N250"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K80" sqref="K80"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" style="33"/>
+    <col min="2" max="2" width="30.28515625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="33" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="33" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="33" customWidth="1"/>
+    <col min="8" max="8" width="29" style="33" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="33" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="33" customWidth="1"/>
+    <col min="11" max="11" width="29" style="33" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="33"/>
+    <col min="13" max="13" width="28.140625" style="33" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" style="33" customWidth="1"/>
+    <col min="15" max="16384" width="16.7109375" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="34">
+        <v>1</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="D5" s="34">
+        <v>100</v>
+      </c>
+      <c r="E5" s="34">
+        <v>1</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="34">
+        <v>2</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" s="34">
+        <v>60</v>
+      </c>
+      <c r="E6" s="34">
+        <v>1</v>
+      </c>
+      <c r="G6" s="34">
+        <v>1</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="J6" s="34">
+        <v>1</v>
+      </c>
+      <c r="K6" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="M6" s="34">
+        <v>1</v>
+      </c>
+      <c r="N6" s="34" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="34">
+        <v>3</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" s="34">
+        <v>80</v>
+      </c>
+      <c r="E7" s="34">
+        <v>1</v>
+      </c>
+      <c r="G7" s="34">
+        <v>2</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="J7" s="34">
+        <v>2</v>
+      </c>
+      <c r="K7" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="M7" s="34">
+        <v>2</v>
+      </c>
+      <c r="N7" s="34" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="34">
+        <v>4</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="D8" s="34">
+        <v>40</v>
+      </c>
+      <c r="E8" s="34">
+        <v>2</v>
+      </c>
+      <c r="G8" s="34">
+        <v>3</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="J8" s="34">
+        <v>3</v>
+      </c>
+      <c r="K8" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="M8" s="34">
+        <v>3</v>
+      </c>
+      <c r="N8" s="34" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34">
+        <v>5</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="D9" s="34">
+        <v>60</v>
+      </c>
+      <c r="E9" s="34">
+        <v>2</v>
+      </c>
+      <c r="G9" s="34">
+        <v>4</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="J9" s="34">
+        <v>4</v>
+      </c>
+      <c r="K9" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="M9" s="34">
+        <v>4</v>
+      </c>
+      <c r="N9" s="34" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="34">
+        <v>6</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" s="34">
+        <v>180</v>
+      </c>
+      <c r="E10" s="34">
+        <v>3</v>
+      </c>
+      <c r="G10" s="34">
+        <v>5</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="J10" s="34">
+        <v>5</v>
+      </c>
+      <c r="K10" s="34" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="34">
+        <v>7</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="34">
+        <v>80</v>
+      </c>
+      <c r="E11" s="34">
+        <v>3</v>
+      </c>
+      <c r="G11" s="34">
+        <v>6</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="J11" s="34">
+        <v>6</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="34">
+        <v>8</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" s="34">
+        <v>126</v>
+      </c>
+      <c r="E12" s="34">
+        <v>3</v>
+      </c>
+      <c r="G12" s="34">
+        <v>7</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="J12" s="34">
+        <v>7</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="34">
+        <v>9</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13" s="34">
+        <v>142</v>
+      </c>
+      <c r="E13" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="34">
+        <v>10</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="34">
+        <v>195</v>
+      </c>
+      <c r="E14" s="34">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="34">
+        <v>11</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" s="34">
+        <v>180</v>
+      </c>
+      <c r="E15" s="34">
+        <v>4</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="34">
+        <v>12</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="D16" s="34">
+        <v>88</v>
+      </c>
+      <c r="E16" s="34">
+        <v>1</v>
+      </c>
+      <c r="G16" s="34">
+        <v>1</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="J16" s="34">
+        <v>1</v>
+      </c>
+      <c r="K16" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="L16" s="34">
+        <v>0</v>
+      </c>
+      <c r="M16" s="34" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="34">
+        <v>13</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D17" s="34">
+        <v>200</v>
+      </c>
+      <c r="E17" s="34">
+        <v>4</v>
+      </c>
+      <c r="G17" s="34">
+        <v>2</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="J17" s="34">
+        <v>2</v>
+      </c>
+      <c r="K17" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="L17" s="34">
+        <v>0</v>
+      </c>
+      <c r="M17" s="34" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="34">
+        <v>14</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="D18" s="34">
+        <v>120</v>
+      </c>
+      <c r="E18" s="34">
+        <v>5</v>
+      </c>
+      <c r="G18" s="34">
+        <v>3</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="J18" s="34">
+        <v>3</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="L18" s="34">
+        <v>0</v>
+      </c>
+      <c r="M18" s="34" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="34">
+        <v>15</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="D19" s="34">
+        <v>160</v>
+      </c>
+      <c r="E19" s="34">
+        <v>5</v>
+      </c>
+      <c r="G19" s="34">
+        <v>4</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="J19" s="34">
+        <v>4</v>
+      </c>
+      <c r="K19" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="34">
+        <v>0</v>
+      </c>
+      <c r="M19" s="34" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="34">
+        <v>16</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="D20" s="34">
+        <v>140</v>
+      </c>
+      <c r="E20" s="34">
+        <v>6</v>
+      </c>
+      <c r="J20" s="34">
+        <v>5</v>
+      </c>
+      <c r="K20" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="L20" s="34">
+        <v>0</v>
+      </c>
+      <c r="M20" s="34" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="34">
+        <v>17</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="D21" s="34">
+        <v>170</v>
+      </c>
+      <c r="E21" s="34">
+        <v>6</v>
+      </c>
+      <c r="J21" s="34">
+        <v>6</v>
+      </c>
+      <c r="K21" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="L21" s="34">
+        <v>1</v>
+      </c>
+      <c r="M21" s="34" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="34">
+        <v>18</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="D22" s="34">
+        <v>120</v>
+      </c>
+      <c r="E22" s="34">
+        <v>5</v>
+      </c>
+      <c r="J22" s="34">
+        <v>7</v>
+      </c>
+      <c r="K22" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="L22" s="34">
+        <v>1</v>
+      </c>
+      <c r="M22" s="34" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="34">
+        <v>19</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="D23" s="34">
+        <v>175</v>
+      </c>
+      <c r="E23" s="34">
+        <v>7</v>
+      </c>
+      <c r="J23" s="34">
+        <v>8</v>
+      </c>
+      <c r="K23" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="L23" s="34">
+        <v>1</v>
+      </c>
+      <c r="M23" s="34" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="34">
+        <v>20</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="D24" s="34">
+        <v>186</v>
+      </c>
+      <c r="E24" s="34">
+        <v>7</v>
+      </c>
+      <c r="J24" s="34">
+        <v>9</v>
+      </c>
+      <c r="K24" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="L24" s="34">
+        <v>1</v>
+      </c>
+      <c r="M24" s="34" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="34">
+        <v>10</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="L25" s="34">
+        <v>1</v>
+      </c>
+      <c r="M25" s="34" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="34">
+        <v>1</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="D29" s="34">
+        <v>20</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="F29" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G29" s="34">
+        <v>0</v>
+      </c>
+      <c r="H29" s="34">
+        <v>1</v>
+      </c>
+      <c r="I29" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="34">
+        <v>2</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="D30" s="34">
+        <v>20</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="F30" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G30" s="34">
+        <v>0</v>
+      </c>
+      <c r="H30" s="34">
+        <v>1</v>
+      </c>
+      <c r="I30" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="34">
+        <v>3</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="D31" s="34">
+        <v>20</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="F31" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G31" s="34">
+        <v>0</v>
+      </c>
+      <c r="H31" s="34">
+        <v>2</v>
+      </c>
+      <c r="I31" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="34">
+        <v>4</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D32" s="34">
+        <v>30</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="F32" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G32" s="34">
+        <v>0</v>
+      </c>
+      <c r="H32" s="34">
+        <v>2</v>
+      </c>
+      <c r="I32" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="34">
+        <v>5</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="D33" s="34">
+        <v>30</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="F33" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G33" s="34">
+        <v>0</v>
+      </c>
+      <c r="H33" s="34">
+        <v>3</v>
+      </c>
+      <c r="I33" s="34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="34">
+        <v>6</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="D34" s="34">
+        <v>40</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="F34" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G34" s="34">
+        <v>0</v>
+      </c>
+      <c r="H34" s="34">
+        <v>3</v>
+      </c>
+      <c r="I34" s="34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="34">
+        <v>7</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="D35" s="34">
+        <v>40</v>
+      </c>
+      <c r="E35" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="F35" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G35" s="34">
+        <v>0</v>
+      </c>
+      <c r="H35" s="34">
+        <v>4</v>
+      </c>
+      <c r="I35" s="34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="34">
+        <v>8</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="D36" s="34">
+        <v>50</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="F36" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G36" s="34">
+        <v>0</v>
+      </c>
+      <c r="H36" s="34">
+        <v>4</v>
+      </c>
+      <c r="I36" s="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="34">
+        <v>9</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="D37" s="34">
+        <v>50</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="F37" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G37" s="34">
+        <v>0</v>
+      </c>
+      <c r="H37" s="34">
+        <v>4</v>
+      </c>
+      <c r="I37" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="34">
+        <v>10</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="D38" s="34">
+        <v>20</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="F38" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G38" s="34">
+        <v>0</v>
+      </c>
+      <c r="H38" s="34">
+        <v>4</v>
+      </c>
+      <c r="I38" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="34">
+        <v>11</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="D39" s="34">
+        <v>30</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="F39" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G39" s="34">
+        <v>0</v>
+      </c>
+      <c r="H39" s="34">
+        <v>3</v>
+      </c>
+      <c r="I39" s="34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="34">
+        <v>12</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="D40" s="34">
+        <v>20</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="F40" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G40" s="34">
+        <v>0</v>
+      </c>
+      <c r="H40" s="34">
+        <v>3</v>
+      </c>
+      <c r="I40" s="34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="34">
+        <v>13</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>309</v>
+      </c>
+      <c r="D41" s="34">
+        <v>40</v>
+      </c>
+      <c r="E41" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="F41" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G41" s="34">
+        <v>0</v>
+      </c>
+      <c r="H41" s="34">
+        <v>1</v>
+      </c>
+      <c r="I41" s="34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="34">
+        <v>1</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="F45" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G45" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="H45" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="34">
+        <v>2</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="E46" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="F46" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G46" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="H46" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="34">
+        <v>3</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="D47" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="E47" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="F47" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G47" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="H47" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="34">
+        <v>4</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="D48" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="E48" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="F48" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G48" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="H48" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="34">
+        <v>5</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="D49" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="F49" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G49" s="34" t="s">
+        <v>293</v>
+      </c>
+      <c r="H49" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="34">
+        <v>6</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="D50" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="E50" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="F50" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G50" s="34" t="s">
+        <v>298</v>
+      </c>
+      <c r="H50" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="34">
+        <v>7</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="F51" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G51" s="34" t="s">
+        <v>294</v>
+      </c>
+      <c r="H51" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="34">
+        <v>8</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="D52" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="E52" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="F52" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G52" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="H52" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="34">
+        <v>9</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="D53" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="E53" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="F53" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G53" s="34" t="s">
+        <v>295</v>
+      </c>
+      <c r="H53" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="34">
+        <v>10</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="D54" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="E54" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="F54" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G54" s="34" t="s">
+        <v>300</v>
+      </c>
+      <c r="H54" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="34">
+        <v>1</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="D58" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E58" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="F58" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G58" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="H58" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="34">
+        <v>2</v>
+      </c>
+      <c r="C59" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>346</v>
+      </c>
+      <c r="E59" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="F59" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G59" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="H59" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="34">
+        <v>3</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="D60" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="F60" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G60" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="H60" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="34">
+        <v>4</v>
+      </c>
+      <c r="C61" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="D61" s="42" t="s">
+        <v>346</v>
+      </c>
+      <c r="E61" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="F61" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G61" s="34" t="s">
+        <v>350</v>
+      </c>
+      <c r="H61" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="34">
+        <v>5</v>
+      </c>
+      <c r="C62" s="34" t="s">
+        <v>339</v>
+      </c>
+      <c r="D62" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E62" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="F62" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G62" s="34" t="s">
+        <v>351</v>
+      </c>
+      <c r="H62" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="34">
+        <v>6</v>
+      </c>
+      <c r="C63" s="34" t="s">
+        <v>340</v>
+      </c>
+      <c r="D63" s="42" t="s">
+        <v>346</v>
+      </c>
+      <c r="E63" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="F63" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G63" s="34" t="s">
+        <v>352</v>
+      </c>
+      <c r="H63" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="34">
+        <v>7</v>
+      </c>
+      <c r="C64" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="D64" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E64" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="F64" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G64" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="H64" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="34">
+        <v>8</v>
+      </c>
+      <c r="C65" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="D65" s="42" t="s">
+        <v>346</v>
+      </c>
+      <c r="E65" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="F65" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G65" s="34" t="s">
+        <v>354</v>
+      </c>
+      <c r="H65" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="34">
+        <v>9</v>
+      </c>
+      <c r="C66" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="D66" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E66" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="F66" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G66" s="34" t="s">
+        <v>355</v>
+      </c>
+      <c r="H66" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="34">
+        <v>10</v>
+      </c>
+      <c r="C67" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="D67" s="42" t="s">
+        <v>346</v>
+      </c>
+      <c r="E67" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="F67" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G67" s="34" t="s">
+        <v>356</v>
+      </c>
+      <c r="H67" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C71" s="32" t="s">
+        <v>357</v>
+      </c>
+      <c r="D71" s="32" t="s">
+        <v>358</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="43" t="s">
+        <v>359</v>
+      </c>
+      <c r="D73" s="43"/>
+      <c r="E73" s="43"/>
+    </row>
+    <row r="74" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
+      <c r="E74" s="43"/>
+    </row>
+    <row r="75" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>361</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="43" t="s">
+        <v>359</v>
+      </c>
+      <c r="D79" s="43"/>
+    </row>
+    <row r="80" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="43"/>
+      <c r="D80" s="43"/>
+    </row>
+    <row r="81" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="C84" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D84" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E84" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C86" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="D86" s="43"/>
+      <c r="E86" s="43"/>
+      <c r="F86" s="43"/>
+    </row>
+    <row r="87" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="43"/>
+      <c r="D87" s="43"/>
+      <c r="E87" s="43"/>
+      <c r="F87" s="43"/>
+    </row>
+    <row r="88" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C88" s="43"/>
+      <c r="D88" s="43"/>
+      <c r="E88" s="43"/>
+      <c r="F88" s="43"/>
+    </row>
+    <row r="89" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="43"/>
+      <c r="D89" s="43"/>
+      <c r="E89" s="43"/>
+      <c r="F89" s="43"/>
+    </row>
+    <row r="90" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="C93" s="45"/>
+    </row>
+    <row r="94" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="43"/>
+      <c r="C94" s="43"/>
+    </row>
+    <row r="95" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="43"/>
+      <c r="C95" s="43"/>
+    </row>
+    <row r="96" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C98" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="45" t="s">
+        <v>364</v>
+      </c>
+      <c r="C99" s="45"/>
+      <c r="D99" s="45"/>
+    </row>
+    <row r="100" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="43"/>
+      <c r="C100" s="43"/>
+      <c r="D100" s="43"/>
+    </row>
+    <row r="101" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="43"/>
+      <c r="C101" s="43"/>
+      <c r="D101" s="43"/>
+    </row>
+    <row r="102" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="46" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="46" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="46" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="46" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C73:E74"/>
+    <mergeCell ref="C79:D80"/>
+    <mergeCell ref="C86:F89"/>
+    <mergeCell ref="B93:C95"/>
+    <mergeCell ref="B99:D101"/>
+  </mergeCells>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D58" r:id="rId1" display="nv11@gmal.com" xr:uid="{7DF6E2BD-3B49-4FAA-B3BB-0FCDE51CAA84}"/>
+    <hyperlink ref="D59" r:id="rId2" xr:uid="{E3901EB7-BB24-429D-AE52-F7883B2B5129}"/>
+    <hyperlink ref="D60" r:id="rId3" display="nv11@gmal.com" xr:uid="{261004D4-3860-43B9-8925-2A22E6E33936}"/>
+    <hyperlink ref="D62" r:id="rId4" display="nv11@gmal.com" xr:uid="{928174DC-5C2E-4225-A85A-8278BBE81D33}"/>
+    <hyperlink ref="D64" r:id="rId5" display="nv11@gmal.com" xr:uid="{2460C548-6DC8-4A27-8305-3CFF55F947A1}"/>
+    <hyperlink ref="D66" r:id="rId6" display="nv11@gmal.com" xr:uid="{6284FDF0-BAC9-4683-8471-9663E68E9EB2}"/>
+    <hyperlink ref="D61" r:id="rId7" xr:uid="{260D9451-C344-4B04-B188-3CC2E8B7889A}"/>
+    <hyperlink ref="D63" r:id="rId8" xr:uid="{1BAB657E-613D-4762-9594-DACCCAEDB43A}"/>
+    <hyperlink ref="D65" r:id="rId9" xr:uid="{98F46F85-1924-4E83-B3E9-1256B52B6BE5}"/>
+    <hyperlink ref="D67" r:id="rId10" xr:uid="{F64156F4-4286-43DA-97CE-4FC776A3E52D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId11"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
LESSON 16 RDBMS - Tao TEST DATA D2 - 04.05.2024
</commit_message>
<xml_diff>
--- a/java21 database design/Java21 QPhan Database Design.xlsx
+++ b/java21 database design/Java21 QPhan Database Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java21\3. Database\java21 database design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E15D668-C3A7-440B-8091-C62DEA68CFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFA4CBE-4282-481B-A318-B926B118B97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="370">
   <si>
     <t>NhanVien</t>
   </si>
@@ -1651,35 +1651,38 @@
     <t>C10_DATE_UNITIL</t>
   </si>
   <si>
+    <t>Sử dụng ITEM ID từ bảng ITEM và fake default path</t>
+  </si>
+  <si>
+    <t>Large amount of data</t>
+  </si>
+  <si>
+    <t>-- 1. Đơn hàng từ 1 - 5 --&gt; Giao thành công (trạng thái từ 1 - 6)</t>
+  </si>
+  <si>
+    <t>-- 2 Đơn hàng từ 6 - 8 --&gt; Đóng gói thành công (trạng thái từ 1 - 4)</t>
+  </si>
+  <si>
+    <t>-- 3. Đơn hàng từ 9 - 10 --&gt; Đang giao hàng (trạng thái từ 1 - 5)</t>
+  </si>
+  <si>
+    <t>-- 4. Đơn hàng từ 11 - 12 --&gt; Hủy đơn hàng (trạng thái 7)</t>
+  </si>
+  <si>
     <t>Sử dụng dữ liệu từ các bảng ITEM, SIZE
 ---
 ITEM, SIZE có ID lẻ: AMOUNT = 125, SALES_PRICE = BUY_PRICE * 2 + SIZE_ID * 5
-ITEM, SIZE có ID lẻ: AMOUNT = 280, SALES_PRICE = BUY_PRICE * 2 + SIZE_ID * 5 + 20</t>
-  </si>
-  <si>
-    <t>Sử dụng ITEM ID từ bảng ITEM và fake default path</t>
-  </si>
-  <si>
-    <t>Large amount of data</t>
-  </si>
-  <si>
-    <t>-- 1. Đơn hàng từ 1 - 5 --&gt; Giao thành công (trạng thái từ 1 - 6)</t>
-  </si>
-  <si>
-    <t>-- 2 Đơn hàng từ 6 - 8 --&gt; Đóng gói thành công (trạng thái từ 1 - 4)</t>
-  </si>
-  <si>
-    <t>-- 3. Đơn hàng từ 9 - 10 --&gt; Đang giao hàng (trạng thái từ 1 - 5)</t>
-  </si>
-  <si>
-    <t>-- 4. Đơn hàng từ 11 - 12 --&gt; Hủy đơn hàng (trạng thái 7)</t>
+ITEM, SIZE có ID chẵn: AMOUNT = 280, SALES_PRICE = BUY_PRICE * 2 + SIZE_ID * 5 + 20</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1834,12 +1837,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -1848,7 +1845,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1864,6 +1861,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1916,9 +1919,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2028,6 +2031,15 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2040,12 +2052,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2055,8 +2061,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3532,7 +3541,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258E744B-65C2-4DE9-994B-E5E54772E544}">
   <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="J11" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="P4" sqref="P4:P8"/>
     </sheetView>
   </sheetViews>
@@ -4014,20 +4023,20 @@
       </c>
     </row>
     <row r="21" spans="2:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G21" s="39" t="s">
+      <c r="G21" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
       <c r="K21" s="1" t="s">
         <v>208</v>
       </c>
@@ -4059,12 +4068,12 @@
       </c>
     </row>
     <row r="23" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="40" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="38"/>
-      <c r="E23" s="38"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
       <c r="F23" s="1">
         <v>1</v>
       </c>
@@ -4108,12 +4117,12 @@
       </c>
     </row>
     <row r="25" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="1">
         <v>3</v>
       </c>
@@ -4157,22 +4166,22 @@
       </c>
     </row>
     <row r="27" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40"/>
+      <c r="E27" s="40"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="38"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="1" t="s">
         <v>173</v>
       </c>
@@ -4180,12 +4189,12 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="2:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="17" t="s">
         <v>174</v>
       </c>
@@ -4421,10 +4430,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8B0AB7-EB07-4BA0-B0D1-595B07C9234C}">
-  <dimension ref="B1:N250"/>
+  <dimension ref="A1:N250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K80" sqref="K80"/>
+    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G107" sqref="G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5686,7 +5695,7 @@
     </row>
     <row r="55" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="47" t="s">
         <v>135</v>
       </c>
     </row>
@@ -5723,7 +5732,7 @@
       <c r="C58" s="34" t="s">
         <v>335</v>
       </c>
-      <c r="D58" s="41" t="s">
+      <c r="D58" s="37" t="s">
         <v>345</v>
       </c>
       <c r="E58" s="34" t="s">
@@ -5746,7 +5755,7 @@
       <c r="C59" s="34" t="s">
         <v>336</v>
       </c>
-      <c r="D59" s="42" t="s">
+      <c r="D59" s="38" t="s">
         <v>346</v>
       </c>
       <c r="E59" s="34" t="s">
@@ -5769,7 +5778,7 @@
       <c r="C60" s="34" t="s">
         <v>338</v>
       </c>
-      <c r="D60" s="41" t="s">
+      <c r="D60" s="37" t="s">
         <v>345</v>
       </c>
       <c r="E60" s="34" t="s">
@@ -5792,7 +5801,7 @@
       <c r="C61" s="34" t="s">
         <v>337</v>
       </c>
-      <c r="D61" s="42" t="s">
+      <c r="D61" s="38" t="s">
         <v>346</v>
       </c>
       <c r="E61" s="34" t="s">
@@ -5815,7 +5824,7 @@
       <c r="C62" s="34" t="s">
         <v>339</v>
       </c>
-      <c r="D62" s="41" t="s">
+      <c r="D62" s="37" t="s">
         <v>345</v>
       </c>
       <c r="E62" s="34" t="s">
@@ -5838,7 +5847,7 @@
       <c r="C63" s="34" t="s">
         <v>340</v>
       </c>
-      <c r="D63" s="42" t="s">
+      <c r="D63" s="38" t="s">
         <v>346</v>
       </c>
       <c r="E63" s="34" t="s">
@@ -5861,7 +5870,7 @@
       <c r="C64" s="34" t="s">
         <v>341</v>
       </c>
-      <c r="D64" s="41" t="s">
+      <c r="D64" s="37" t="s">
         <v>345</v>
       </c>
       <c r="E64" s="34" t="s">
@@ -5884,7 +5893,7 @@
       <c r="C65" s="34" t="s">
         <v>342</v>
       </c>
-      <c r="D65" s="42" t="s">
+      <c r="D65" s="38" t="s">
         <v>346</v>
       </c>
       <c r="E65" s="34" t="s">
@@ -5907,7 +5916,7 @@
       <c r="C66" s="34" t="s">
         <v>343</v>
       </c>
-      <c r="D66" s="41" t="s">
+      <c r="D66" s="37" t="s">
         <v>345</v>
       </c>
       <c r="E66" s="34" t="s">
@@ -5930,7 +5939,7 @@
       <c r="C67" s="34" t="s">
         <v>344</v>
       </c>
-      <c r="D67" s="42" t="s">
+      <c r="D67" s="38" t="s">
         <v>346</v>
       </c>
       <c r="E67" s="34" t="s">
@@ -5949,7 +5958,7 @@
     <row r="68" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="69" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="70" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="47" t="s">
         <v>137</v>
       </c>
     </row>
@@ -5972,20 +5981,20 @@
     </row>
     <row r="72" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C73" s="43" t="s">
+      <c r="C73" s="44" t="s">
         <v>359</v>
       </c>
-      <c r="D73" s="43"/>
-      <c r="E73" s="43"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
     </row>
     <row r="74" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C74" s="43"/>
-      <c r="D74" s="43"/>
-      <c r="E74" s="43"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="44"/>
+      <c r="E74" s="44"/>
     </row>
     <row r="75" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="76" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="47" t="s">
         <v>138</v>
       </c>
     </row>
@@ -6005,14 +6014,14 @@
     </row>
     <row r="78" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="79" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="43" t="s">
+      <c r="C79" s="44" t="s">
         <v>359</v>
       </c>
-      <c r="D79" s="43"/>
+      <c r="D79" s="44"/>
     </row>
     <row r="80" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="43"/>
-      <c r="D80" s="43"/>
+      <c r="C80" s="44"/>
+      <c r="D80" s="44"/>
     </row>
     <row r="81" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6022,7 +6031,7 @@
       </c>
     </row>
     <row r="84" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B84" s="31" t="s">
+      <c r="B84" s="15" t="s">
         <v>168</v>
       </c>
       <c r="C84" s="20" t="s">
@@ -6043,34 +6052,34 @@
     </row>
     <row r="85" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="86" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C86" s="44" t="s">
-        <v>362</v>
-      </c>
-      <c r="D86" s="43"/>
-      <c r="E86" s="43"/>
-      <c r="F86" s="43"/>
+      <c r="C86" s="45" t="s">
+        <v>368</v>
+      </c>
+      <c r="D86" s="44"/>
+      <c r="E86" s="44"/>
+      <c r="F86" s="44"/>
     </row>
     <row r="87" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="43"/>
-      <c r="D87" s="43"/>
-      <c r="E87" s="43"/>
-      <c r="F87" s="43"/>
+      <c r="C87" s="44"/>
+      <c r="D87" s="44"/>
+      <c r="E87" s="44"/>
+      <c r="F87" s="44"/>
     </row>
     <row r="88" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C88" s="43"/>
-      <c r="D88" s="43"/>
-      <c r="E88" s="43"/>
-      <c r="F88" s="43"/>
+      <c r="C88" s="44"/>
+      <c r="D88" s="44"/>
+      <c r="E88" s="44"/>
+      <c r="F88" s="44"/>
     </row>
     <row r="89" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C89" s="43"/>
-      <c r="D89" s="43"/>
-      <c r="E89" s="43"/>
-      <c r="F89" s="43"/>
+      <c r="C89" s="44"/>
+      <c r="D89" s="44"/>
+      <c r="E89" s="44"/>
+      <c r="F89" s="44"/>
     </row>
     <row r="90" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="16" t="s">
+      <c r="B91" s="47" t="s">
         <v>149</v>
       </c>
     </row>
@@ -6083,26 +6092,26 @@
       </c>
     </row>
     <row r="93" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="45" t="s">
-        <v>363</v>
-      </c>
-      <c r="C93" s="45"/>
+      <c r="B93" s="46" t="s">
+        <v>362</v>
+      </c>
+      <c r="C93" s="46"/>
     </row>
     <row r="94" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="43"/>
-      <c r="C94" s="43"/>
+      <c r="B94" s="44"/>
+      <c r="C94" s="44"/>
     </row>
     <row r="95" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="43"/>
-      <c r="C95" s="43"/>
+      <c r="B95" s="44"/>
+      <c r="C95" s="44"/>
     </row>
     <row r="96" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="25" t="s">
+    <row r="97" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="48" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="98" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="15" t="s">
         <v>166</v>
       </c>
@@ -6113,30 +6122,33 @@
         <v>167</v>
       </c>
     </row>
-    <row r="99" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="45" t="s">
-        <v>364</v>
-      </c>
-      <c r="C99" s="45"/>
-      <c r="D99" s="45"/>
-    </row>
-    <row r="100" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="43"/>
-      <c r="C100" s="43"/>
-      <c r="D100" s="43"/>
-    </row>
-    <row r="101" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="43"/>
-      <c r="C101" s="43"/>
-      <c r="D101" s="43"/>
-    </row>
-    <row r="102" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B103" s="16" t="s">
+    <row r="99" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="46" t="s">
+        <v>363</v>
+      </c>
+      <c r="C99" s="46"/>
+      <c r="D99" s="46"/>
+    </row>
+    <row r="100" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="44"/>
+      <c r="C100" s="44"/>
+      <c r="D100" s="44"/>
+    </row>
+    <row r="101" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="44"/>
+      <c r="C101" s="44"/>
+      <c r="D101" s="44"/>
+    </row>
+    <row r="102" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="33" t="s">
+        <v>369</v>
+      </c>
+      <c r="B103" s="47" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="104" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B104" s="15" t="s">
         <v>174</v>
       </c>
@@ -6150,30 +6162,30 @@
         <v>228</v>
       </c>
     </row>
-    <row r="105" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="46" t="s">
+    <row r="105" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="39" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="39" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="107" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="46" t="s">
+    <row r="108" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="39" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="108" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="46" t="s">
+    <row r="109" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="39" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="109" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="46" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="110" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="113" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="114" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="115" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
LESSON16 - RDBMS - Database Design 07.05.2024
</commit_message>
<xml_diff>
--- a/java21 database design/Java21 QPhan Database Design.xlsx
+++ b/java21 database design/Java21 QPhan Database Design.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\TAILIEU\java21\3.DATABASE\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java21\3. Database\java21 database design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F60483-B17B-4E6C-8936-21716132D968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E15D668-C3A7-440B-8091-C62DEA68CFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
     <sheet name="B2. Mô hình logic" sheetId="2" r:id="rId2"/>
     <sheet name="B3. Mô hình vật lý" sheetId="4" r:id="rId3"/>
+    <sheet name="Bn. Tạo dữ liệu kiểm thử" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -174,6 +175,9 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={8EC58335-C900-492B-BA28-EE6A8C506FC5}</author>
+    <author>Quyen Ngoc Phan</author>
+    <author>tc={34745E4D-1BCF-46E0-8BDB-A445EE5E1BD2}</author>
+    <author>tc={C1921E78-7869-444A-8472-B8D666CCBAC5}</author>
     <author>tc={1305DD5C-A913-487C-8B38-59BD0DFB2D0F}</author>
     <author>tc={F01BC811-4E6C-4543-AA25-E955BE8491CD}</author>
     <author>tc={3702AC3F-ACCB-4FA5-81F8-3D4343E0ECEF}</author>
@@ -193,7 +197,73 @@
     Không cần thuộc phòng ban, làm được mọi chức năng</t>
       </text>
     </comment>
-    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{1305DD5C-A913-487C-8B38-59BD0DFB2D0F}">
+    <comment ref="K4" authorId="1" shapeId="0" xr:uid="{B746EB97-6D3C-4F53-97FC-412D4E572F20}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Bảng doanh thu, lưu doanh thu bán hàng từ ngày from đến ngày until số tiền bao nhiêu
+Chưa xử lý lưu trữ danh sách mặt hàng, đơn hàng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E6" authorId="2" shapeId="0" xr:uid="{34745E4D-1BCF-46E0-8BDB-A445EE5E1BD2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Tiền mặt, thẻ tín dụng, thẻ ghi nợ, ví điện tử</t>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="3" shapeId="0" xr:uid="{C1921E78-7869-444A-8472-B8D666CCBAC5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Chờ xác nhận, Đang đóng gói, Đóng gói hoàn thành chờ vận chuyển, Đang vận chuyển, Giao hàng thành công, Giao hàng thất bại, Hủy đơn hàng</t>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="1" shapeId="0" xr:uid="{BFDAA607-05E3-4FA6-9169-4193A867187B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Lưu KDL DATE
+VD: 25/03 --&gt; tương ứng với ngày 25/03 0H0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="4" shapeId="0" xr:uid="{1305DD5C-A913-487C-8B38-59BD0DFB2D0F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -201,7 +271,33 @@
     Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</t>
       </text>
     </comment>
-    <comment ref="J8" authorId="2" shapeId="0" xr:uid="{F01BC811-4E6C-4543-AA25-E955BE8491CD}">
+    <comment ref="J7" authorId="1" shapeId="0" xr:uid="{464FAC46-B928-4D1B-B9FC-CA444F74AF8B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Lưu KDL DATE
+VD: 28/03 --&gt; tương ứng với ngày 28/3 23H59H59
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="5" shapeId="0" xr:uid="{F01BC811-4E6C-4543-AA25-E955BE8491CD}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -210,7 +306,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="M8" authorId="3" shapeId="0" xr:uid="{3702AC3F-ACCB-4FA5-81F8-3D4343E0ECEF}">
+    <comment ref="M8" authorId="6" shapeId="0" xr:uid="{3702AC3F-ACCB-4FA5-81F8-3D4343E0ECEF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -218,7 +314,7 @@
     Có rất nhiều màu sắc color, rgb, hexa -&gt; sử dụng varchar để lưu chứ k tạo 1 bảng riêng</t>
       </text>
     </comment>
-    <comment ref="J9" authorId="4" shapeId="0" xr:uid="{9527FEF5-CCFC-4F64-97A2-BBE2E29C2803}">
+    <comment ref="J9" authorId="7" shapeId="0" xr:uid="{9527FEF5-CCFC-4F64-97A2-BBE2E29C2803}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -226,7 +322,7 @@
     How - tính số lượng tồn kho theo giai đoạn ?</t>
       </text>
     </comment>
-    <comment ref="K9" authorId="5" shapeId="0" xr:uid="{3DE62A8D-5F5B-409E-A562-B1F200B29412}">
+    <comment ref="K9" authorId="8" shapeId="0" xr:uid="{3DE62A8D-5F5B-409E-A562-B1F200B29412}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -234,7 +330,7 @@
     Lưu thông tin bán những mặt hàng nào số lượng bao nhiêu, JSON, OBJECT</t>
       </text>
     </comment>
-    <comment ref="J10" authorId="6" shapeId="0" xr:uid="{43CCAF04-133F-49FE-87EB-557285BF8E90}">
+    <comment ref="J10" authorId="9" shapeId="0" xr:uid="{43CCAF04-133F-49FE-87EB-557285BF8E90}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -242,7 +338,7 @@
     Doanh thu cho mặt hàng theo giai đoạn</t>
       </text>
     </comment>
-    <comment ref="M10" authorId="7" shapeId="0" xr:uid="{2853FC81-A62F-4574-A1AA-7A29E9B44A89}">
+    <comment ref="M10" authorId="10" shapeId="0" xr:uid="{2853FC81-A62F-4574-A1AA-7A29E9B44A89}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -250,7 +346,7 @@
     Số lượng hàng còn lại ở thời điểm hiện tại</t>
       </text>
     </comment>
-    <comment ref="H12" authorId="8" shapeId="0" xr:uid="{B9E52DF8-6EBC-4DCF-8C8A-1994D6E5BB03}">
+    <comment ref="H12" authorId="11" shapeId="0" xr:uid="{B9E52DF8-6EBC-4DCF-8C8A-1994D6E5BB03}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -258,7 +354,7 @@
     NhanVien, Quan Ly</t>
       </text>
     </comment>
-    <comment ref="I22" authorId="9" shapeId="0" xr:uid="{4B47AF2D-C770-4A5E-8158-147A119469B1}">
+    <comment ref="I22" authorId="12" shapeId="0" xr:uid="{4B47AF2D-C770-4A5E-8158-147A119469B1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -270,8 +366,176 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={3503BA87-F97B-4BA2-B285-74026B5E7BB4}</author>
+    <author>tc={F417F53F-78F4-4FB2-9932-6B06E3741ADD}</author>
+    <author>tc={73A9844D-439C-4A34-96F0-71631781CCF8}</author>
+    <author>tc={89D0F75C-16FA-43DB-9BE0-099B1CAFC699}</author>
+    <author>tc={81011C5D-5AE3-44B3-97CD-014DF419A278}</author>
+    <author>Quyen Ngoc Phan</author>
+    <author>tc={D45AF084-4675-422C-9958-D87148145BEA}</author>
+    <author>tc={BFF9823B-C3B1-4818-99DA-2E82CF873073}</author>
+    <author>tc={AE19BEC5-BB6C-4F20-A9C5-16CD0C497F85}</author>
+    <author>tc={686C344B-1B7B-4A75-97B6-A6A7B29739FE}</author>
+  </authors>
+  <commentList>
+    <comment ref="D4" authorId="0" shapeId="0" xr:uid="{3503BA87-F97B-4BA2-B285-74026B5E7BB4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</t>
+      </text>
+    </comment>
+    <comment ref="K5" authorId="1" shapeId="0" xr:uid="{F417F53F-78F4-4FB2-9932-6B06E3741ADD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Chờ xác nhận, Đang đóng gói, Đóng gói hoàn thành chờ vận chuyển, Đang vận chuyển, Giao hàng thành công, Giao hàng thất bại, Hủy đơn hàng</t>
+      </text>
+    </comment>
+    <comment ref="H15" authorId="2" shapeId="0" xr:uid="{73A9844D-439C-4A34-96F0-71631781CCF8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Tiền mặt, thẻ tín dụng, thẻ ghi nợ, ví điện tử</t>
+      </text>
+    </comment>
+    <comment ref="B56" authorId="3" shapeId="0" xr:uid="{89D0F75C-16FA-43DB-9BE0-099B1CAFC699}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Không cần thuộc phòng ban, làm được mọi chức năng</t>
+      </text>
+    </comment>
+    <comment ref="I57" authorId="4" shapeId="0" xr:uid="{81011C5D-5AE3-44B3-97CD-014DF419A278}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NhanVien, Quan Ly</t>
+      </text>
+    </comment>
+    <comment ref="C71" authorId="5" shapeId="0" xr:uid="{97B38917-3C27-42E5-A452-A7A63273C962}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Lưu KDL DATE
+VD: 25/03 --&gt; tương ứng với ngày 25/03 0H0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D71" authorId="5" shapeId="0" xr:uid="{89BC852F-A852-42D9-8A07-73738E7D49A8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Lưu KDL DATE
+VD: 28/03 --&gt; tương ứng với ngày 28/3 23H59H59
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E71" authorId="6" shapeId="0" xr:uid="{D45AF084-4675-422C-9958-D87148145BEA}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Số lượng bán
+</t>
+      </text>
+    </comment>
+    <comment ref="F71" authorId="7" shapeId="0" xr:uid="{BFF9823B-C3B1-4818-99DA-2E82CF873073}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Doanh thu cho mặt hàng theo giai đoạn</t>
+      </text>
+    </comment>
+    <comment ref="B76" authorId="5" shapeId="0" xr:uid="{3308BC73-AD5E-408B-A255-F1435759065A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Quyen Ngoc Phan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Bảng doanh thu, lưu doanh thu bán hàng từ ngày from đến ngày until số tiền bao nhiêu
+Chưa xử lý lưu trữ danh sách mặt hàng, đơn hàng</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E84" authorId="8" shapeId="0" xr:uid="{AE19BEC5-BB6C-4F20-A9C5-16CD0C497F85}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Có rất nhiều màu sắc color, rgb, hexa -&gt; sử dụng varchar để lưu chứ k tạo 1 bảng riêng</t>
+      </text>
+    </comment>
+    <comment ref="G84" authorId="9" shapeId="0" xr:uid="{686C344B-1B7B-4A75-97B6-A6A7B29739FE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Số lượng hàng còn lại ở thời điểm hiện tại</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="369">
   <si>
     <t>NhanVien</t>
   </si>
@@ -901,6 +1165,9 @@
     <t>C07_TITLE_ID</t>
   </si>
   <si>
+    <t>C08_TITLE_ID</t>
+  </si>
+  <si>
     <t>C08_TITLE_NAME</t>
   </si>
   <si>
@@ -928,9 +1195,6 @@
     <t>C09_REVENUE</t>
   </si>
   <si>
-    <t>C09_DATE_UNITIL 23:59</t>
-  </si>
-  <si>
     <t>C09_DATE_FROM 00:00</t>
   </si>
   <si>
@@ -958,18 +1222,6 @@
     <t>C11_CUSTOMER_EMAIL</t>
   </si>
   <si>
-    <t>C11_EMPLOYEE_ADDRESS</t>
-  </si>
-  <si>
-    <t>C11_EMPLOYEE_PHONE</t>
-  </si>
-  <si>
-    <t>C11_EMPLOYEE_USERNAME</t>
-  </si>
-  <si>
-    <t>C11_EMPLOYEE_PASSWORD</t>
-  </si>
-  <si>
     <t>Mô hình logic trên cơ sở đối tượng ==&gt; https://app.diagrams.net/#G1EC3kWNgwWJ-jrYKf-W24OTGjAV-pxvRf#%7B%22pageId%22%3A%22AbEYu_0bn73_d0lKOqK0%22%7D</t>
   </si>
   <si>
@@ -982,14 +1234,452 @@
     <t>Lưu ý: Bản cuối cùng tạm thời của phần thiết kế</t>
   </si>
   <si>
-    <t>X`</t>
+    <t>C09_DATE_UNTIL 23:59:59</t>
+  </si>
+  <si>
+    <t>C11_CUSTOMER_ADDRESS</t>
+  </si>
+  <si>
+    <t>C11_CUSTOMER_PHONE</t>
+  </si>
+  <si>
+    <t>C11_CUSTOMER_USERNAME</t>
+  </si>
+  <si>
+    <t>C11_CUSTOMER_PASSWORD</t>
+  </si>
+  <si>
+    <t>C15_LAST_UPDATED</t>
+  </si>
+  <si>
+    <t>[from, until]</t>
+  </si>
+  <si>
+    <t>Áo</t>
+  </si>
+  <si>
+    <t>Quần</t>
+  </si>
+  <si>
+    <t>Giày</t>
+  </si>
+  <si>
+    <t>Dép</t>
+  </si>
+  <si>
+    <t>Mũ</t>
+  </si>
+  <si>
+    <t>Thắt lưng</t>
+  </si>
+  <si>
+    <t>Túi xách</t>
+  </si>
+  <si>
+    <t>Áo 1</t>
+  </si>
+  <si>
+    <t>Áo 2</t>
+  </si>
+  <si>
+    <t>Áo 3</t>
+  </si>
+  <si>
+    <t>Quần 4</t>
+  </si>
+  <si>
+    <t>Quần 5</t>
+  </si>
+  <si>
+    <t>Giày 6</t>
+  </si>
+  <si>
+    <t>Giày 7</t>
+  </si>
+  <si>
+    <t>Giày 8</t>
+  </si>
+  <si>
+    <t>Giày 9</t>
+  </si>
+  <si>
+    <t>Giày 10</t>
+  </si>
+  <si>
+    <t>Giép 11</t>
+  </si>
+  <si>
+    <t>Áo 12</t>
+  </si>
+  <si>
+    <t>Giép 13</t>
+  </si>
+  <si>
+    <t>Mũ 14</t>
+  </si>
+  <si>
+    <t>Mũ 15</t>
+  </si>
+  <si>
+    <t>Thắt lưng 16</t>
+  </si>
+  <si>
+    <t>Thắt lưng 17</t>
+  </si>
+  <si>
+    <t>Mũ 18</t>
+  </si>
+  <si>
+    <t>Túi xách 1</t>
+  </si>
+  <si>
+    <t>Túi xách 2</t>
+  </si>
+  <si>
+    <t>Tiền mặt</t>
+  </si>
+  <si>
+    <t>Thẻ tín dụng</t>
+  </si>
+  <si>
+    <t>Thẻ ghi nợ</t>
+  </si>
+  <si>
+    <t>Ví điện tử</t>
+  </si>
+  <si>
+    <t>c1@gmal.com</t>
+  </si>
+  <si>
+    <t>c2@gmal.com</t>
+  </si>
+  <si>
+    <t>c3@gmal.com</t>
+  </si>
+  <si>
+    <t>c4@gmal.com</t>
+  </si>
+  <si>
+    <t>c5@gmal.com</t>
+  </si>
+  <si>
+    <t>c6@gmal.com</t>
+  </si>
+  <si>
+    <t>c7@gmal.com</t>
+  </si>
+  <si>
+    <t>c8@gmal.com</t>
+  </si>
+  <si>
+    <t>c9@gmal.com</t>
+  </si>
+  <si>
+    <t>c10@gmal.com</t>
+  </si>
+  <si>
+    <t>Lê Tèo</t>
+  </si>
+  <si>
+    <t>Văn An</t>
+  </si>
+  <si>
+    <t>Nguyễn A</t>
+  </si>
+  <si>
+    <t>Phan Tuấn</t>
+  </si>
+  <si>
+    <t>Hoàng Tiên</t>
+  </si>
+  <si>
+    <t>Phạm Ngọc</t>
+  </si>
+  <si>
+    <t>Đoạn Tú</t>
+  </si>
+  <si>
+    <t>Hoàng B</t>
+  </si>
+  <si>
+    <t>Lê Huân</t>
+  </si>
+  <si>
+    <t>Nam Ban</t>
+  </si>
+  <si>
+    <t>Địa chỉ 1</t>
+  </si>
+  <si>
+    <t>Địa chỉ 2</t>
+  </si>
+  <si>
+    <t>Địa chỉ 3</t>
+  </si>
+  <si>
+    <t>Địa chỉ 4</t>
+  </si>
+  <si>
+    <t>Địa chỉ 5</t>
+  </si>
+  <si>
+    <t>Địa chỉ 6</t>
+  </si>
+  <si>
+    <t>Địa chỉ 7</t>
+  </si>
+  <si>
+    <t>Địa chỉ 8</t>
+  </si>
+  <si>
+    <t>Địa chỉ 9</t>
+  </si>
+  <si>
+    <t>Địa chỉ 10</t>
+  </si>
+  <si>
+    <t>c1def</t>
+  </si>
+  <si>
+    <t>c3def</t>
+  </si>
+  <si>
+    <t>c5def</t>
+  </si>
+  <si>
+    <t>c7def</t>
+  </si>
+  <si>
+    <t>c9def</t>
+  </si>
+  <si>
+    <t>c2auto</t>
+  </si>
+  <si>
+    <t>c4auto</t>
+  </si>
+  <si>
+    <t>c6auto</t>
+  </si>
+  <si>
+    <t>c8auto</t>
+  </si>
+  <si>
+    <t>c10auto</t>
+  </si>
+  <si>
+    <t>$2a$12$w0bs0MW/O3nTyMhuv0r1jOjq2gOaxLxkZgms7u/khHRmtCh3S/Hpu</t>
+  </si>
+  <si>
+    <t>10.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>12.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>14.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>16.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>18.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>20.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>26.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>28.04.2024 08:10:20</t>
+  </si>
+  <si>
+    <t>Địa chỉ 11</t>
+  </si>
+  <si>
+    <t>Địa chỉ 12</t>
+  </si>
+  <si>
+    <t>Địa chỉ 13</t>
+  </si>
+  <si>
+    <t>Dùng công thức để tính</t>
+  </si>
+  <si>
+    <t>Chờ xác nhận</t>
+  </si>
+  <si>
+    <t>Đang đóng gói</t>
+  </si>
+  <si>
+    <t>Đóng gói hoàn thành</t>
+  </si>
+  <si>
+    <t>Đang vận chuyển</t>
+  </si>
+  <si>
+    <t>Giao hàng thành công</t>
+  </si>
+  <si>
+    <t>Giao hàng thất bại</t>
+  </si>
+  <si>
+    <t>Hủy đơn hàng</t>
+  </si>
+  <si>
+    <t>Size 'S' cho Nữ</t>
+  </si>
+  <si>
+    <t>Size 'M' cho Nữ</t>
+  </si>
+  <si>
+    <t>Size 'L' cho Nữ</t>
+  </si>
+  <si>
+    <t>Size 'XL' cho Nữ</t>
+  </si>
+  <si>
+    <t>Size 'XXL' cho Nữ</t>
+  </si>
+  <si>
+    <t>Size 'S' cho Nam</t>
+  </si>
+  <si>
+    <t>Size 'M' cho Nam</t>
+  </si>
+  <si>
+    <t>Size 'L' cho Nam</t>
+  </si>
+  <si>
+    <t>Size 'XL' cho Nam</t>
+  </si>
+  <si>
+    <t>Size 'XXL' cho Nam</t>
+  </si>
+  <si>
+    <t>Nhân viên</t>
+  </si>
+  <si>
+    <t>Trưởng bộ phận</t>
+  </si>
+  <si>
+    <t>Chủ sở hữu</t>
+  </si>
+  <si>
+    <t>Giảm đốc</t>
+  </si>
+  <si>
+    <t>Nhân viên 1</t>
+  </si>
+  <si>
+    <t>Nhân viên 2</t>
+  </si>
+  <si>
+    <t>Nhân viên 4</t>
+  </si>
+  <si>
+    <t>Nhân viên 3</t>
+  </si>
+  <si>
+    <t>Nhân viên 5</t>
+  </si>
+  <si>
+    <t>Nhân viên 6</t>
+  </si>
+  <si>
+    <t>Nhân viên 7</t>
+  </si>
+  <si>
+    <t>Nhân viên 8</t>
+  </si>
+  <si>
+    <t>Nhân viên 9</t>
+  </si>
+  <si>
+    <t>Nhân viên 10</t>
+  </si>
+  <si>
+    <t>nv1@gmal.com</t>
+  </si>
+  <si>
+    <t>nv2@gmal.com</t>
+  </si>
+  <si>
+    <t>nv1def</t>
+  </si>
+  <si>
+    <t>nv2auto</t>
+  </si>
+  <si>
+    <t>nv3def</t>
+  </si>
+  <si>
+    <t>nv4auto</t>
+  </si>
+  <si>
+    <t>nv5def</t>
+  </si>
+  <si>
+    <t>nv6auto</t>
+  </si>
+  <si>
+    <t>nv7def</t>
+  </si>
+  <si>
+    <t>nv8auto</t>
+  </si>
+  <si>
+    <t>nv9def</t>
+  </si>
+  <si>
+    <t>nv10auto</t>
+  </si>
+  <si>
+    <t>C09_DATE_FROM</t>
+  </si>
+  <si>
+    <t>C09_DATE_UNTIL</t>
+  </si>
+  <si>
+    <t>Bài tập phần DML - Tạo câu truy vấn để xử lý</t>
+  </si>
+  <si>
+    <t>C10_DATE_FROM</t>
+  </si>
+  <si>
+    <t>C10_DATE_UNITIL</t>
+  </si>
+  <si>
+    <t>Sử dụng dữ liệu từ các bảng ITEM, SIZE
+---
+ITEM, SIZE có ID lẻ: AMOUNT = 125, SALES_PRICE = BUY_PRICE * 2 + SIZE_ID * 5
+ITEM, SIZE có ID lẻ: AMOUNT = 280, SALES_PRICE = BUY_PRICE * 2 + SIZE_ID * 5 + 20</t>
+  </si>
+  <si>
+    <t>Sử dụng ITEM ID từ bảng ITEM và fake default path</t>
+  </si>
+  <si>
+    <t>Large amount of data</t>
+  </si>
+  <si>
+    <t>-- 1. Đơn hàng từ 1 - 5 --&gt; Giao thành công (trạng thái từ 1 - 6)</t>
+  </si>
+  <si>
+    <t>-- 2 Đơn hàng từ 6 - 8 --&gt; Đóng gói thành công (trạng thái từ 1 - 4)</t>
+  </si>
+  <si>
+    <t>-- 3. Đơn hàng từ 9 - 10 --&gt; Đang giao hàng (trạng thái từ 1 - 5)</t>
+  </si>
+  <si>
+    <t>-- 4. Đơn hàng từ 11 - 12 --&gt; Hủy đơn hàng (trạng thái 7)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1111,10 +1801,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="12"/>
-      <color rgb="FFC00000"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1140,7 +1868,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1176,11 +1904,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1266,9 +2004,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1278,8 +2013,20 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1288,10 +2035,32 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1631,6 +2400,12 @@
   <threadedComment ref="H4" dT="2024-03-19T13:48:38.72" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{8EC58335-C900-492B-BA28-EE6A8C506FC5}">
     <text>Không cần thuộc phòng ban, làm được mọi chức năng</text>
   </threadedComment>
+  <threadedComment ref="E6" dT="2024-04-06T14:23:17.00" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{34745E4D-1BCF-46E0-8BDB-A445EE5E1BD2}">
+    <text>Tiền mặt, thẻ tín dụng, thẻ ghi nợ, ví điện tử</text>
+  </threadedComment>
+  <threadedComment ref="F6" dT="2024-04-06T14:25:21.49" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{C1921E78-7869-444A-8472-B8D666CCBAC5}">
+    <text>Chờ xác nhận, Đang đóng gói, Đóng gói hoàn thành chờ vận chuyển, Đang vận chuyển, Giao hàng thành công, Giao hàng thất bại, Hủy đơn hàng</text>
+  </threadedComment>
   <threadedComment ref="B7" dT="2024-03-19T12:47:34.71" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{1305DD5C-A913-487C-8B38-59BD0DFB2D0F}">
     <text>Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</text>
   </threadedComment>
@@ -1662,6 +2437,39 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment4.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D4" dT="2024-03-19T12:47:34.71" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{3503BA87-F97B-4BA2-B285-74026B5E7BB4}">
+    <text>Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</text>
+  </threadedComment>
+  <threadedComment ref="K5" dT="2024-04-06T14:25:21.49" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{F417F53F-78F4-4FB2-9932-6B06E3741ADD}">
+    <text>Chờ xác nhận, Đang đóng gói, Đóng gói hoàn thành chờ vận chuyển, Đang vận chuyển, Giao hàng thành công, Giao hàng thất bại, Hủy đơn hàng</text>
+  </threadedComment>
+  <threadedComment ref="H15" dT="2024-04-06T14:23:17.00" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{73A9844D-439C-4A34-96F0-71631781CCF8}">
+    <text>Tiền mặt, thẻ tín dụng, thẻ ghi nợ, ví điện tử</text>
+  </threadedComment>
+  <threadedComment ref="B56" dT="2024-03-19T13:48:38.72" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{89D0F75C-16FA-43DB-9BE0-099B1CAFC699}">
+    <text>Không cần thuộc phòng ban, làm được mọi chức năng</text>
+  </threadedComment>
+  <threadedComment ref="I57" dT="2024-03-19T13:49:56.69" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{81011C5D-5AE3-44B3-97CD-014DF419A278}">
+    <text>NhanVien, Quan Ly</text>
+  </threadedComment>
+  <threadedComment ref="E71" dT="2024-04-02T13:49:52.63" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{D45AF084-4675-422C-9958-D87148145BEA}">
+    <text xml:space="preserve">Số lượng bán
+</text>
+  </threadedComment>
+  <threadedComment ref="F71" dT="2024-04-02T13:55:15.51" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{BFF9823B-C3B1-4818-99DA-2E82CF873073}">
+    <text>Doanh thu cho mặt hàng theo giai đoạn</text>
+  </threadedComment>
+  <threadedComment ref="E84" dT="2024-04-02T12:50:53.71" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{AE19BEC5-BB6C-4F20-A9C5-16CD0C497F85}">
+    <text>Có rất nhiều màu sắc color, rgb, hexa -&gt; sử dụng varchar để lưu chứ k tạo 1 bảng riêng</text>
+  </threadedComment>
+  <threadedComment ref="G84" dT="2024-04-02T13:53:18.17" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{686C344B-1B7B-4A75-97B6-A6A7B29739FE}">
+    <text>Số lượng hàng còn lại ở thời điểm hiện tại</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L35"/>
@@ -1670,35 +2478,35 @@
       <selection activeCell="B24" sqref="B24:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="1" customWidth="1"/>
-    <col min="3" max="4" width="14.6640625" style="1" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="23" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" style="1" customWidth="1"/>
-    <col min="8" max="9" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="1" customWidth="1"/>
-    <col min="12" max="29" width="14.6640625" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.109375" style="1"/>
+    <col min="12" max="29" width="14.7109375" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1733,7 +2541,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
@@ -1768,7 +2576,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>35</v>
       </c>
@@ -1803,7 +2611,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1830,7 +2638,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1855,7 +2663,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
@@ -1878,7 +2686,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
@@ -1901,7 +2709,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
@@ -1924,7 +2732,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>15</v>
       </c>
@@ -1942,7 +2750,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
@@ -1959,7 +2767,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
@@ -1976,7 +2784,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -1991,7 +2799,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -2003,7 +2811,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2016,7 +2824,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2029,8 +2837,8 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
@@ -2038,7 +2846,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>37</v>
       </c>
@@ -2046,7 +2854,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>38</v>
       </c>
@@ -2054,24 +2862,24 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="1" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="1" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="1" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2083,39 +2891,39 @@
   <dimension ref="B1:L35"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.109375" style="1" customWidth="1"/>
-    <col min="8" max="9" width="14.6640625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="1" customWidth="1"/>
     <col min="11" max="11" width="20" style="1" customWidth="1"/>
-    <col min="12" max="29" width="14.6640625" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.109375" style="1"/>
+    <col min="12" max="29" width="14.7109375" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="2" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>36</v>
       </c>
@@ -2150,7 +2958,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
@@ -2185,7 +2993,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
@@ -2220,7 +3028,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
@@ -2255,7 +3063,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>10</v>
       </c>
@@ -2282,7 +3090,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
@@ -2309,7 +3117,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
@@ -2332,7 +3140,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
@@ -2355,7 +3163,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
@@ -2378,7 +3186,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>61</v>
       </c>
@@ -2396,7 +3204,7 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
@@ -2412,7 +3220,7 @@
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -2427,7 +3235,7 @@
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -2442,7 +3250,7 @@
       <c r="K15" s="3"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -2455,7 +3263,7 @@
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
     </row>
-    <row r="17" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2468,7 +3276,7 @@
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2481,8 +3289,8 @@
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
     </row>
-    <row r="19" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
         <v>57</v>
       </c>
@@ -2490,7 +3298,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>58</v>
       </c>
@@ -2513,7 +3321,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>59</v>
       </c>
@@ -2536,7 +3344,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>60</v>
       </c>
@@ -2559,7 +3367,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G24" s="1">
         <v>3</v>
       </c>
@@ -2579,7 +3387,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
         <v>73</v>
       </c>
@@ -2602,7 +3410,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>74</v>
       </c>
@@ -2613,7 +3421,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>75</v>
       </c>
@@ -2627,7 +3435,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>76</v>
       </c>
@@ -2641,7 +3449,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H29" s="1" t="s">
         <v>67</v>
       </c>
@@ -2649,12 +3457,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>80</v>
       </c>
@@ -2671,7 +3479,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" s="1" t="s">
         <v>83</v>
       </c>
@@ -2685,7 +3493,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="5:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="5:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" s="1" t="s">
         <v>83</v>
       </c>
@@ -2699,7 +3507,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="5:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="5:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="1" t="s">
         <v>83</v>
       </c>
@@ -2713,7 +3521,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="5:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="5:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2724,47 +3532,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258E744B-65C2-4DE9-994B-E5E54772E544}">
   <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="H1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4:P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="33.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="27.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="27" style="1" customWidth="1"/>
-    <col min="12" max="12" width="30.5546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="22.6640625" style="1" customWidth="1"/>
-    <col min="15" max="15" width="22.33203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="28.6640625" style="1" customWidth="1"/>
-    <col min="17" max="29" width="14.6640625" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="9.109375" style="1"/>
+    <col min="12" max="12" width="30.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="28.7109375" style="1" customWidth="1"/>
+    <col min="17" max="29" width="14.7109375" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="2" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
-        <v>225</v>
-      </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -2773,11 +3581,13 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
+      <c r="J3" s="6" t="s">
+        <v>229</v>
+      </c>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
     </row>
-    <row r="4" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>122</v>
       </c>
@@ -2824,7 +3634,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
         <v>128</v>
       </c>
@@ -2847,18 +3657,18 @@
         <v>192</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="J5" s="29" t="s">
-        <v>201</v>
-      </c>
-      <c r="K5" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="K5" s="15" t="s">
         <v>211</v>
       </c>
       <c r="L5" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="31" t="s">
         <v>168</v>
       </c>
       <c r="N5" s="15" t="s">
@@ -2871,7 +3681,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>130</v>
       </c>
@@ -2894,15 +3704,15 @@
         <v>193</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="J6" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="J6" s="32" t="s">
         <v>210</v>
       </c>
       <c r="K6" s="15" t="s">
         <v>212</v>
       </c>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="3" t="s">
         <v>217</v>
       </c>
       <c r="M6" s="20" t="s">
@@ -2911,14 +3721,14 @@
       <c r="N6" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="O6" s="31" t="s">
         <v>170</v>
       </c>
       <c r="P6" s="15" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>129</v>
       </c>
@@ -2935,8 +3745,8 @@
         <v>194</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="15" t="s">
-        <v>209</v>
+      <c r="J7" s="32" t="s">
+        <v>223</v>
       </c>
       <c r="K7" s="15" t="s">
         <v>214</v>
@@ -2955,7 +3765,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>152</v>
       </c>
@@ -2973,13 +3783,13 @@
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>213</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="M8" s="20" t="s">
         <v>144</v>
@@ -2987,10 +3797,10 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
@@ -3004,13 +3814,13 @@
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="28" t="s">
-        <v>203</v>
-      </c>
-      <c r="K9" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="K9" s="30" t="s">
         <v>215</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>220</v>
+        <v>225</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>142</v>
@@ -3019,7 +3829,7 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
@@ -3033,11 +3843,11 @@
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="K10" s="31"/>
-      <c r="L10" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
+      </c>
+      <c r="K10" s="30"/>
+      <c r="L10" s="20" t="s">
+        <v>226</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>148</v>
@@ -3046,7 +3856,7 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
       <c r="D11" s="4" t="s">
@@ -3058,17 +3868,18 @@
       <c r="H11" s="3" t="s">
         <v>198</v>
       </c>
+      <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="4"/>
       <c r="C12" s="3"/>
       <c r="D12" s="4" t="s">
@@ -3080,7 +3891,7 @@
       <c r="H12" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="I12" s="30"/>
+      <c r="I12" s="29"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
@@ -3089,16 +3900,15 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="30"/>
+      <c r="H13" s="29"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
       <c r="M13" s="3"/>
@@ -3106,7 +3916,7 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -3123,9 +3933,9 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
-      <c r="C15" s="30"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
@@ -3134,16 +3944,16 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="30"/>
+      <c r="L15" s="29"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="30"/>
+      <c r="D16" s="29"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -3157,7 +3967,7 @@
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
     </row>
-    <row r="17" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -3174,7 +3984,7 @@
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -3191,41 +4001,41 @@
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11" t="s">
         <v>100</v>
       </c>
       <c r="K20" s="27" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="34" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="37"/>
       <c r="F21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G21" s="33" t="s">
+      <c r="G21" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
       <c r="K21" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="L21" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
         <v>101</v>
       </c>
@@ -3248,13 +4058,13 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="34" t="s">
+    <row r="23" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
       <c r="F23" s="1">
         <v>1</v>
       </c>
@@ -3274,7 +4084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="11" t="s">
         <v>104</v>
       </c>
@@ -3297,13 +4107,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="34" t="s">
+    <row r="25" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="36"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
       <c r="F25" s="1">
         <v>3</v>
       </c>
@@ -3323,7 +4133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
         <v>106</v>
       </c>
@@ -3346,36 +4156,36 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="34" t="s">
+    <row r="27" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="37" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="34" t="s">
+    <row r="28" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
+      <c r="C28" s="38"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="1" t="s">
         <v>173</v>
       </c>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="2:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="34" t="s">
+    <row r="29" spans="2:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="17" t="s">
         <v>174</v>
       </c>
@@ -3389,7 +4199,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="30" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F30" s="6">
         <v>77</v>
       </c>
@@ -3400,7 +4210,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="31" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F31" s="6">
         <v>77</v>
       </c>
@@ -3411,7 +4221,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="32" spans="2:16" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="12" t="s">
         <v>110</v>
       </c>
@@ -3425,7 +4235,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="33" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>111</v>
       </c>
@@ -3439,7 +4249,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="34" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
         <v>112</v>
       </c>
@@ -3455,7 +4265,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="35" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>113</v>
       </c>
@@ -3469,30 +4279,30 @@
         <v>183</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>116</v>
       </c>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>114</v>
       </c>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
         <v>115</v>
       </c>
@@ -3501,24 +4311,24 @@
       <c r="E41" s="11"/>
       <c r="F41" s="11"/>
     </row>
-    <row r="42" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
         <v>124</v>
       </c>
@@ -3526,7 +4336,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="48" spans="2:8" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
         <v>126</v>
       </c>
@@ -3534,9 +4344,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="13" t="s">
         <v>184</v>
       </c>
@@ -3545,7 +4355,7 @@
       <c r="E51" s="13"/>
       <c r="F51" s="13"/>
     </row>
-    <row r="52" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="26" t="s">
         <v>185</v>
       </c>
@@ -3554,21 +4364,21 @@
       <c r="E52" s="13"/>
       <c r="F52" s="13"/>
     </row>
-    <row r="53" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B53" s="13"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
       <c r="E53" s="13"/>
       <c r="F53" s="13"/>
     </row>
-    <row r="54" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B54" s="13"/>
       <c r="C54" s="13"/>
       <c r="D54" s="13"/>
       <c r="E54" s="13"/>
       <c r="F54" s="13"/>
     </row>
-    <row r="55" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55" s="13" t="s">
         <v>186</v>
       </c>
@@ -3577,7 +4387,7 @@
       <c r="E55" s="13"/>
       <c r="F55" s="13"/>
     </row>
-    <row r="56" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56" s="26" t="s">
         <v>187</v>
       </c>
@@ -3586,17 +4396,16 @@
       <c r="E56" s="13"/>
       <c r="F56" s="13"/>
     </row>
-    <row r="57" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="2:6" ht="21.9" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B2:E2"/>
+  <mergeCells count="7">
     <mergeCell ref="B29:E29"/>
     <mergeCell ref="G21:I21"/>
     <mergeCell ref="B21:E21"/>
@@ -3608,4 +4417,1923 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8B0AB7-EB07-4BA0-B0D1-595B07C9234C}">
+  <dimension ref="B1:N250"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K80" sqref="K80"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" style="33"/>
+    <col min="2" max="2" width="30.28515625" style="33" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="33" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="33" customWidth="1"/>
+    <col min="7" max="7" width="32.5703125" style="33" customWidth="1"/>
+    <col min="8" max="8" width="29" style="33" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" style="33" customWidth="1"/>
+    <col min="10" max="10" width="25.28515625" style="33" customWidth="1"/>
+    <col min="11" max="11" width="29" style="33" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" style="33"/>
+    <col min="13" max="13" width="28.140625" style="33" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" style="33" customWidth="1"/>
+    <col min="15" max="16384" width="16.7109375" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="34">
+        <v>1</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="D5" s="34">
+        <v>100</v>
+      </c>
+      <c r="E5" s="34">
+        <v>1</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="34">
+        <v>2</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="D6" s="34">
+        <v>60</v>
+      </c>
+      <c r="E6" s="34">
+        <v>1</v>
+      </c>
+      <c r="G6" s="34">
+        <v>1</v>
+      </c>
+      <c r="H6" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="J6" s="34">
+        <v>1</v>
+      </c>
+      <c r="K6" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="M6" s="34">
+        <v>1</v>
+      </c>
+      <c r="N6" s="34" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="34">
+        <v>3</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" s="34">
+        <v>80</v>
+      </c>
+      <c r="E7" s="34">
+        <v>1</v>
+      </c>
+      <c r="G7" s="34">
+        <v>2</v>
+      </c>
+      <c r="H7" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="J7" s="34">
+        <v>2</v>
+      </c>
+      <c r="K7" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="M7" s="34">
+        <v>2</v>
+      </c>
+      <c r="N7" s="34" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="34">
+        <v>4</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>240</v>
+      </c>
+      <c r="D8" s="34">
+        <v>40</v>
+      </c>
+      <c r="E8" s="34">
+        <v>2</v>
+      </c>
+      <c r="G8" s="34">
+        <v>3</v>
+      </c>
+      <c r="H8" s="34" t="s">
+        <v>232</v>
+      </c>
+      <c r="J8" s="34">
+        <v>3</v>
+      </c>
+      <c r="K8" s="34" t="s">
+        <v>316</v>
+      </c>
+      <c r="M8" s="34">
+        <v>3</v>
+      </c>
+      <c r="N8" s="34" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="34">
+        <v>5</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>241</v>
+      </c>
+      <c r="D9" s="34">
+        <v>60</v>
+      </c>
+      <c r="E9" s="34">
+        <v>2</v>
+      </c>
+      <c r="G9" s="34">
+        <v>4</v>
+      </c>
+      <c r="H9" s="34" t="s">
+        <v>233</v>
+      </c>
+      <c r="J9" s="34">
+        <v>4</v>
+      </c>
+      <c r="K9" s="34" t="s">
+        <v>317</v>
+      </c>
+      <c r="M9" s="34">
+        <v>4</v>
+      </c>
+      <c r="N9" s="34" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="34">
+        <v>6</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>242</v>
+      </c>
+      <c r="D10" s="34">
+        <v>180</v>
+      </c>
+      <c r="E10" s="34">
+        <v>3</v>
+      </c>
+      <c r="G10" s="34">
+        <v>5</v>
+      </c>
+      <c r="H10" s="34" t="s">
+        <v>234</v>
+      </c>
+      <c r="J10" s="34">
+        <v>5</v>
+      </c>
+      <c r="K10" s="34" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="34">
+        <v>7</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="34">
+        <v>80</v>
+      </c>
+      <c r="E11" s="34">
+        <v>3</v>
+      </c>
+      <c r="G11" s="34">
+        <v>6</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="J11" s="34">
+        <v>6</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="34">
+        <v>8</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>244</v>
+      </c>
+      <c r="D12" s="34">
+        <v>126</v>
+      </c>
+      <c r="E12" s="34">
+        <v>3</v>
+      </c>
+      <c r="G12" s="34">
+        <v>7</v>
+      </c>
+      <c r="H12" s="34" t="s">
+        <v>236</v>
+      </c>
+      <c r="J12" s="34">
+        <v>7</v>
+      </c>
+      <c r="K12" s="34" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="34">
+        <v>9</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>245</v>
+      </c>
+      <c r="D13" s="34">
+        <v>142</v>
+      </c>
+      <c r="E13" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="34">
+        <v>10</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>246</v>
+      </c>
+      <c r="D14" s="34">
+        <v>195</v>
+      </c>
+      <c r="E14" s="34">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="34">
+        <v>11</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" s="34">
+        <v>180</v>
+      </c>
+      <c r="E15" s="34">
+        <v>4</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="34">
+        <v>12</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="D16" s="34">
+        <v>88</v>
+      </c>
+      <c r="E16" s="34">
+        <v>1</v>
+      </c>
+      <c r="G16" s="34">
+        <v>1</v>
+      </c>
+      <c r="H16" s="34" t="s">
+        <v>257</v>
+      </c>
+      <c r="J16" s="34">
+        <v>1</v>
+      </c>
+      <c r="K16" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="L16" s="34">
+        <v>0</v>
+      </c>
+      <c r="M16" s="34" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="34">
+        <v>13</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="D17" s="34">
+        <v>200</v>
+      </c>
+      <c r="E17" s="34">
+        <v>4</v>
+      </c>
+      <c r="G17" s="34">
+        <v>2</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>258</v>
+      </c>
+      <c r="J17" s="34">
+        <v>2</v>
+      </c>
+      <c r="K17" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="L17" s="34">
+        <v>0</v>
+      </c>
+      <c r="M17" s="34" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="34">
+        <v>14</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>250</v>
+      </c>
+      <c r="D18" s="34">
+        <v>120</v>
+      </c>
+      <c r="E18" s="34">
+        <v>5</v>
+      </c>
+      <c r="G18" s="34">
+        <v>3</v>
+      </c>
+      <c r="H18" s="34" t="s">
+        <v>259</v>
+      </c>
+      <c r="J18" s="34">
+        <v>3</v>
+      </c>
+      <c r="K18" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="L18" s="34">
+        <v>0</v>
+      </c>
+      <c r="M18" s="34" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="34">
+        <v>15</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>251</v>
+      </c>
+      <c r="D19" s="34">
+        <v>160</v>
+      </c>
+      <c r="E19" s="34">
+        <v>5</v>
+      </c>
+      <c r="G19" s="34">
+        <v>4</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>260</v>
+      </c>
+      <c r="J19" s="34">
+        <v>4</v>
+      </c>
+      <c r="K19" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="L19" s="34">
+        <v>0</v>
+      </c>
+      <c r="M19" s="34" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="34">
+        <v>16</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>252</v>
+      </c>
+      <c r="D20" s="34">
+        <v>140</v>
+      </c>
+      <c r="E20" s="34">
+        <v>6</v>
+      </c>
+      <c r="J20" s="34">
+        <v>5</v>
+      </c>
+      <c r="K20" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="L20" s="34">
+        <v>0</v>
+      </c>
+      <c r="M20" s="34" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="34">
+        <v>17</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>253</v>
+      </c>
+      <c r="D21" s="34">
+        <v>170</v>
+      </c>
+      <c r="E21" s="34">
+        <v>6</v>
+      </c>
+      <c r="J21" s="34">
+        <v>6</v>
+      </c>
+      <c r="K21" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="L21" s="34">
+        <v>1</v>
+      </c>
+      <c r="M21" s="34" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="34">
+        <v>18</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>254</v>
+      </c>
+      <c r="D22" s="34">
+        <v>120</v>
+      </c>
+      <c r="E22" s="34">
+        <v>5</v>
+      </c>
+      <c r="J22" s="34">
+        <v>7</v>
+      </c>
+      <c r="K22" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="L22" s="34">
+        <v>1</v>
+      </c>
+      <c r="M22" s="34" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="34">
+        <v>19</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>255</v>
+      </c>
+      <c r="D23" s="34">
+        <v>175</v>
+      </c>
+      <c r="E23" s="34">
+        <v>7</v>
+      </c>
+      <c r="J23" s="34">
+        <v>8</v>
+      </c>
+      <c r="K23" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="L23" s="34">
+        <v>1</v>
+      </c>
+      <c r="M23" s="34" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="34">
+        <v>20</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>256</v>
+      </c>
+      <c r="D24" s="34">
+        <v>186</v>
+      </c>
+      <c r="E24" s="34">
+        <v>7</v>
+      </c>
+      <c r="J24" s="34">
+        <v>9</v>
+      </c>
+      <c r="K24" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="L24" s="34">
+        <v>1</v>
+      </c>
+      <c r="M24" s="34" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J25" s="34">
+        <v>10</v>
+      </c>
+      <c r="K25" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="L25" s="34">
+        <v>1</v>
+      </c>
+      <c r="M25" s="34" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="G27" s="33" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="34">
+        <v>1</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>302</v>
+      </c>
+      <c r="D29" s="34">
+        <v>20</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="F29" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G29" s="34">
+        <v>0</v>
+      </c>
+      <c r="H29" s="34">
+        <v>1</v>
+      </c>
+      <c r="I29" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="34">
+        <v>2</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="D30" s="34">
+        <v>20</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="F30" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G30" s="34">
+        <v>0</v>
+      </c>
+      <c r="H30" s="34">
+        <v>1</v>
+      </c>
+      <c r="I30" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="34">
+        <v>3</v>
+      </c>
+      <c r="C31" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="D31" s="34">
+        <v>20</v>
+      </c>
+      <c r="E31" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="F31" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G31" s="34">
+        <v>0</v>
+      </c>
+      <c r="H31" s="34">
+        <v>2</v>
+      </c>
+      <c r="I31" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="34">
+        <v>4</v>
+      </c>
+      <c r="C32" s="35" t="s">
+        <v>305</v>
+      </c>
+      <c r="D32" s="34">
+        <v>30</v>
+      </c>
+      <c r="E32" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="F32" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G32" s="34">
+        <v>0</v>
+      </c>
+      <c r="H32" s="34">
+        <v>2</v>
+      </c>
+      <c r="I32" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="34">
+        <v>5</v>
+      </c>
+      <c r="C33" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="D33" s="34">
+        <v>30</v>
+      </c>
+      <c r="E33" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="F33" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G33" s="34">
+        <v>0</v>
+      </c>
+      <c r="H33" s="34">
+        <v>3</v>
+      </c>
+      <c r="I33" s="34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="34">
+        <v>6</v>
+      </c>
+      <c r="C34" s="35" t="s">
+        <v>303</v>
+      </c>
+      <c r="D34" s="34">
+        <v>40</v>
+      </c>
+      <c r="E34" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="F34" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G34" s="34">
+        <v>0</v>
+      </c>
+      <c r="H34" s="34">
+        <v>3</v>
+      </c>
+      <c r="I34" s="34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="34">
+        <v>7</v>
+      </c>
+      <c r="C35" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="D35" s="34">
+        <v>40</v>
+      </c>
+      <c r="E35" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="F35" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G35" s="34">
+        <v>0</v>
+      </c>
+      <c r="H35" s="34">
+        <v>4</v>
+      </c>
+      <c r="I35" s="34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="34">
+        <v>8</v>
+      </c>
+      <c r="C36" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="D36" s="34">
+        <v>50</v>
+      </c>
+      <c r="E36" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="F36" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G36" s="34">
+        <v>0</v>
+      </c>
+      <c r="H36" s="34">
+        <v>4</v>
+      </c>
+      <c r="I36" s="34">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="34">
+        <v>9</v>
+      </c>
+      <c r="C37" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="D37" s="34">
+        <v>50</v>
+      </c>
+      <c r="E37" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="F37" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G37" s="34">
+        <v>0</v>
+      </c>
+      <c r="H37" s="34">
+        <v>4</v>
+      </c>
+      <c r="I37" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="34">
+        <v>10</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>306</v>
+      </c>
+      <c r="D38" s="34">
+        <v>20</v>
+      </c>
+      <c r="E38" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="F38" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G38" s="34">
+        <v>0</v>
+      </c>
+      <c r="H38" s="34">
+        <v>4</v>
+      </c>
+      <c r="I38" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="34">
+        <v>11</v>
+      </c>
+      <c r="C39" s="35" t="s">
+        <v>307</v>
+      </c>
+      <c r="D39" s="34">
+        <v>30</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>310</v>
+      </c>
+      <c r="F39" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G39" s="34">
+        <v>0</v>
+      </c>
+      <c r="H39" s="34">
+        <v>3</v>
+      </c>
+      <c r="I39" s="34">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="34">
+        <v>12</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>308</v>
+      </c>
+      <c r="D40" s="34">
+        <v>20</v>
+      </c>
+      <c r="E40" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="F40" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G40" s="34">
+        <v>0</v>
+      </c>
+      <c r="H40" s="34">
+        <v>3</v>
+      </c>
+      <c r="I40" s="34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="34">
+        <v>13</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>309</v>
+      </c>
+      <c r="D41" s="34">
+        <v>40</v>
+      </c>
+      <c r="E41" s="34" t="s">
+        <v>312</v>
+      </c>
+      <c r="F41" s="34">
+        <v>258369741</v>
+      </c>
+      <c r="G41" s="34">
+        <v>0</v>
+      </c>
+      <c r="H41" s="34">
+        <v>1</v>
+      </c>
+      <c r="I41" s="34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="34">
+        <v>1</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>271</v>
+      </c>
+      <c r="D45" s="35" t="s">
+        <v>261</v>
+      </c>
+      <c r="E45" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="F45" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G45" s="34" t="s">
+        <v>291</v>
+      </c>
+      <c r="H45" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="34">
+        <v>2</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>272</v>
+      </c>
+      <c r="D46" s="34" t="s">
+        <v>262</v>
+      </c>
+      <c r="E46" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="F46" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G46" s="34" t="s">
+        <v>296</v>
+      </c>
+      <c r="H46" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="34">
+        <v>3</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>273</v>
+      </c>
+      <c r="D47" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="E47" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="F47" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G47" s="34" t="s">
+        <v>292</v>
+      </c>
+      <c r="H47" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="34">
+        <v>4</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>274</v>
+      </c>
+      <c r="D48" s="34" t="s">
+        <v>264</v>
+      </c>
+      <c r="E48" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="F48" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G48" s="34" t="s">
+        <v>297</v>
+      </c>
+      <c r="H48" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="34">
+        <v>5</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="D49" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="E49" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="F49" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G49" s="34" t="s">
+        <v>293</v>
+      </c>
+      <c r="H49" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="34">
+        <v>6</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>276</v>
+      </c>
+      <c r="D50" s="34" t="s">
+        <v>266</v>
+      </c>
+      <c r="E50" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="F50" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G50" s="34" t="s">
+        <v>298</v>
+      </c>
+      <c r="H50" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="34">
+        <v>7</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="D51" s="34" t="s">
+        <v>267</v>
+      </c>
+      <c r="E51" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="F51" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G51" s="34" t="s">
+        <v>294</v>
+      </c>
+      <c r="H51" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="34">
+        <v>8</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>278</v>
+      </c>
+      <c r="D52" s="34" t="s">
+        <v>268</v>
+      </c>
+      <c r="E52" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="F52" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G52" s="34" t="s">
+        <v>299</v>
+      </c>
+      <c r="H52" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="34">
+        <v>9</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>279</v>
+      </c>
+      <c r="D53" s="34" t="s">
+        <v>269</v>
+      </c>
+      <c r="E53" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="F53" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G53" s="34" t="s">
+        <v>295</v>
+      </c>
+      <c r="H53" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="34">
+        <v>10</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>280</v>
+      </c>
+      <c r="D54" s="34" t="s">
+        <v>270</v>
+      </c>
+      <c r="E54" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="F54" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G54" s="34" t="s">
+        <v>300</v>
+      </c>
+      <c r="H54" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="58" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="34">
+        <v>1</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>335</v>
+      </c>
+      <c r="D58" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E58" s="34" t="s">
+        <v>281</v>
+      </c>
+      <c r="F58" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G58" s="34" t="s">
+        <v>347</v>
+      </c>
+      <c r="H58" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="34">
+        <v>2</v>
+      </c>
+      <c r="C59" s="34" t="s">
+        <v>336</v>
+      </c>
+      <c r="D59" s="42" t="s">
+        <v>346</v>
+      </c>
+      <c r="E59" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="F59" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G59" s="34" t="s">
+        <v>348</v>
+      </c>
+      <c r="H59" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="34">
+        <v>3</v>
+      </c>
+      <c r="C60" s="34" t="s">
+        <v>338</v>
+      </c>
+      <c r="D60" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E60" s="34" t="s">
+        <v>283</v>
+      </c>
+      <c r="F60" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G60" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="H60" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="34">
+        <v>4</v>
+      </c>
+      <c r="C61" s="34" t="s">
+        <v>337</v>
+      </c>
+      <c r="D61" s="42" t="s">
+        <v>346</v>
+      </c>
+      <c r="E61" s="34" t="s">
+        <v>284</v>
+      </c>
+      <c r="F61" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G61" s="34" t="s">
+        <v>350</v>
+      </c>
+      <c r="H61" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="34">
+        <v>5</v>
+      </c>
+      <c r="C62" s="34" t="s">
+        <v>339</v>
+      </c>
+      <c r="D62" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E62" s="34" t="s">
+        <v>285</v>
+      </c>
+      <c r="F62" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G62" s="34" t="s">
+        <v>351</v>
+      </c>
+      <c r="H62" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="63" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="34">
+        <v>6</v>
+      </c>
+      <c r="C63" s="34" t="s">
+        <v>340</v>
+      </c>
+      <c r="D63" s="42" t="s">
+        <v>346</v>
+      </c>
+      <c r="E63" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="F63" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G63" s="34" t="s">
+        <v>352</v>
+      </c>
+      <c r="H63" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="34">
+        <v>7</v>
+      </c>
+      <c r="C64" s="34" t="s">
+        <v>341</v>
+      </c>
+      <c r="D64" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E64" s="34" t="s">
+        <v>287</v>
+      </c>
+      <c r="F64" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G64" s="34" t="s">
+        <v>353</v>
+      </c>
+      <c r="H64" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="34">
+        <v>8</v>
+      </c>
+      <c r="C65" s="34" t="s">
+        <v>342</v>
+      </c>
+      <c r="D65" s="42" t="s">
+        <v>346</v>
+      </c>
+      <c r="E65" s="34" t="s">
+        <v>288</v>
+      </c>
+      <c r="F65" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G65" s="34" t="s">
+        <v>354</v>
+      </c>
+      <c r="H65" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="34">
+        <v>9</v>
+      </c>
+      <c r="C66" s="34" t="s">
+        <v>343</v>
+      </c>
+      <c r="D66" s="41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E66" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="F66" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G66" s="34" t="s">
+        <v>355</v>
+      </c>
+      <c r="H66" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="34">
+        <v>10</v>
+      </c>
+      <c r="C67" s="34" t="s">
+        <v>344</v>
+      </c>
+      <c r="D67" s="42" t="s">
+        <v>346</v>
+      </c>
+      <c r="E67" s="34" t="s">
+        <v>290</v>
+      </c>
+      <c r="F67" s="34">
+        <v>123456789</v>
+      </c>
+      <c r="G67" s="34" t="s">
+        <v>356</v>
+      </c>
+      <c r="H67" s="36" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="C71" s="32" t="s">
+        <v>357</v>
+      </c>
+      <c r="D71" s="32" t="s">
+        <v>358</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="43" t="s">
+        <v>359</v>
+      </c>
+      <c r="D73" s="43"/>
+      <c r="E73" s="43"/>
+    </row>
+    <row r="74" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
+      <c r="E74" s="43"/>
+    </row>
+    <row r="75" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="C77" s="15" t="s">
+        <v>360</v>
+      </c>
+      <c r="D77" s="15" t="s">
+        <v>361</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="43" t="s">
+        <v>359</v>
+      </c>
+      <c r="D79" s="43"/>
+    </row>
+    <row r="80" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="43"/>
+      <c r="D80" s="43"/>
+    </row>
+    <row r="81" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="C84" s="20" t="s">
+        <v>141</v>
+      </c>
+      <c r="D84" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="E84" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C86" s="44" t="s">
+        <v>362</v>
+      </c>
+      <c r="D86" s="43"/>
+      <c r="E86" s="43"/>
+      <c r="F86" s="43"/>
+    </row>
+    <row r="87" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="43"/>
+      <c r="D87" s="43"/>
+      <c r="E87" s="43"/>
+      <c r="F87" s="43"/>
+    </row>
+    <row r="88" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C88" s="43"/>
+      <c r="D88" s="43"/>
+      <c r="E88" s="43"/>
+      <c r="F88" s="43"/>
+    </row>
+    <row r="89" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="43"/>
+      <c r="D89" s="43"/>
+      <c r="E89" s="43"/>
+      <c r="F89" s="43"/>
+    </row>
+    <row r="90" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B92" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B93" s="45" t="s">
+        <v>363</v>
+      </c>
+      <c r="C93" s="45"/>
+    </row>
+    <row r="94" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="43"/>
+      <c r="C94" s="43"/>
+    </row>
+    <row r="95" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="43"/>
+      <c r="C95" s="43"/>
+    </row>
+    <row r="96" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="25" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="98" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B98" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C98" s="31" t="s">
+        <v>170</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="99" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="45" t="s">
+        <v>364</v>
+      </c>
+      <c r="C99" s="45"/>
+      <c r="D99" s="45"/>
+    </row>
+    <row r="100" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="43"/>
+      <c r="C100" s="43"/>
+      <c r="D100" s="43"/>
+    </row>
+    <row r="101" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="43"/>
+      <c r="C101" s="43"/>
+      <c r="D101" s="43"/>
+    </row>
+    <row r="102" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="104" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C104" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="105" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="46" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="107" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="46" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="108" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="46" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="109" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="46" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="110" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C73:E74"/>
+    <mergeCell ref="C79:D80"/>
+    <mergeCell ref="C86:F89"/>
+    <mergeCell ref="B93:C95"/>
+    <mergeCell ref="B99:D101"/>
+  </mergeCells>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D58" r:id="rId1" display="nv11@gmal.com" xr:uid="{7DF6E2BD-3B49-4FAA-B3BB-0FCDE51CAA84}"/>
+    <hyperlink ref="D59" r:id="rId2" xr:uid="{E3901EB7-BB24-429D-AE52-F7883B2B5129}"/>
+    <hyperlink ref="D60" r:id="rId3" display="nv11@gmal.com" xr:uid="{261004D4-3860-43B9-8925-2A22E6E33936}"/>
+    <hyperlink ref="D62" r:id="rId4" display="nv11@gmal.com" xr:uid="{928174DC-5C2E-4225-A85A-8278BBE81D33}"/>
+    <hyperlink ref="D64" r:id="rId5" display="nv11@gmal.com" xr:uid="{2460C548-6DC8-4A27-8305-3CFF55F947A1}"/>
+    <hyperlink ref="D66" r:id="rId6" display="nv11@gmal.com" xr:uid="{6284FDF0-BAC9-4683-8471-9663E68E9EB2}"/>
+    <hyperlink ref="D61" r:id="rId7" xr:uid="{260D9451-C344-4B04-B188-3CC2E8B7889A}"/>
+    <hyperlink ref="D63" r:id="rId8" xr:uid="{1BAB657E-613D-4762-9594-DACCCAEDB43A}"/>
+    <hyperlink ref="D65" r:id="rId9" xr:uid="{98F46F85-1924-4E83-B3E9-1256B52B6BE5}"/>
+    <hyperlink ref="D67" r:id="rId10" xr:uid="{F64156F4-4286-43DA-97CE-4FC776A3E52D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId11"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finish creating test data - 11.05.2024
</commit_message>
<xml_diff>
--- a/java21 database design/Java21 QPhan Database Design.xlsx
+++ b/java21 database design/Java21 QPhan Database Design.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java21\3. Database\java21 database design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFA4CBE-4282-481B-A318-B926B118B97F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD3F05A-3704-4745-AEB0-4247B5A1EDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1965" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="384">
   <si>
     <t>NhanVien</t>
   </si>
@@ -1567,9 +1567,6 @@
     <t>Chủ sở hữu</t>
   </si>
   <si>
-    <t>Giảm đốc</t>
-  </si>
-  <si>
     <t>Nhân viên 1</t>
   </si>
   <si>
@@ -1655,15 +1652,6 @@
   </si>
   <si>
     <t>Large amount of data</t>
-  </si>
-  <si>
-    <t>-- 1. Đơn hàng từ 1 - 5 --&gt; Giao thành công (trạng thái từ 1 - 6)</t>
-  </si>
-  <si>
-    <t>-- 2 Đơn hàng từ 6 - 8 --&gt; Đóng gói thành công (trạng thái từ 1 - 4)</t>
-  </si>
-  <si>
-    <t>-- 3. Đơn hàng từ 9 - 10 --&gt; Đang giao hàng (trạng thái từ 1 - 5)</t>
   </si>
   <si>
     <t>-- 4. Đơn hàng từ 11 - 12 --&gt; Hủy đơn hàng (trạng thái 7)</t>
@@ -1675,14 +1663,68 @@
 ITEM, SIZE có ID chẵn: AMOUNT = 280, SALES_PRICE = BUY_PRICE * 2 + SIZE_ID * 5 + 20</t>
   </si>
   <si>
-    <t>x</t>
+    <t>nv3@gmal.com</t>
+  </si>
+  <si>
+    <t>nv4@gmal.com</t>
+  </si>
+  <si>
+    <t>nv6@gmal.com</t>
+  </si>
+  <si>
+    <t>nv7@gmal.com</t>
+  </si>
+  <si>
+    <t>nv8@gmal.com</t>
+  </si>
+  <si>
+    <t>nv9@gmal.com</t>
+  </si>
+  <si>
+    <t>nv10@gmal.com</t>
+  </si>
+  <si>
+    <t>nv5@gmail.com</t>
+  </si>
+  <si>
+    <t>Giám đốc</t>
+  </si>
+  <si>
+    <t>Fake 100 rows</t>
+  </si>
+  <si>
+    <t>Nhân Viên 2</t>
+  </si>
+  <si>
+    <t>Nhân Viên 3</t>
+  </si>
+  <si>
+    <t>Nhân Viên 4</t>
+  </si>
+  <si>
+    <t>-- 1. Đơn hàng từ 1 - 5 --&gt; Giao thành công (trạng thái từ 1 - 5)</t>
+  </si>
+  <si>
+    <t>-- 2 Đơn hàng từ 6 - 8 --&gt; Đóng gói thành công (trạng thái từ 1 - 3)</t>
+  </si>
+  <si>
+    <t>-- 3. Đơn hàng từ 9 - 10 --&gt; Đang giao hàng (trạng thái từ 1 - 4)</t>
+  </si>
+  <si>
+    <t>Nhân Viên 5</t>
+  </si>
+  <si>
+    <t>SYSDATE - max(STATUS_ID) - ORDER_STATUS_ID</t>
+  </si>
+  <si>
+    <t>-- 4. Đơn hàng từ 13  --&gt; Giao hàng thất bại (trạng thái 1,2,3,4,6)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1836,16 +1878,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1867,6 +1901,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1917,9 +1957,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2031,14 +2070,17 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2061,15 +2103,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3541,8 +3579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258E744B-65C2-4DE9-994B-E5E54772E544}">
   <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView topLeftCell="J11" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4:P8"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4023,20 +4061,20 @@
       </c>
     </row>
     <row r="21" spans="2:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="40"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
       <c r="F21" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="G21" s="42" t="s">
+      <c r="G21" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
       <c r="K21" s="1" t="s">
         <v>208</v>
       </c>
@@ -4068,12 +4106,12 @@
       </c>
     </row>
     <row r="23" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="41" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
       <c r="F23" s="1">
         <v>1</v>
       </c>
@@ -4117,12 +4155,12 @@
       </c>
     </row>
     <row r="25" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="40" t="s">
+      <c r="B25" s="41" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="44"/>
       <c r="F25" s="1">
         <v>3</v>
       </c>
@@ -4166,22 +4204,22 @@
       </c>
     </row>
     <row r="27" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="40" t="s">
+      <c r="B27" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
     <row r="28" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="40" t="s">
+      <c r="B28" s="41" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
       <c r="F28" s="1" t="s">
         <v>173</v>
       </c>
@@ -4189,12 +4227,12 @@
       <c r="K28" s="7"/>
     </row>
     <row r="29" spans="2:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="40" t="s">
+      <c r="B29" s="41" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
+      <c r="C29" s="42"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="42"/>
       <c r="F29" s="17" t="s">
         <v>174</v>
       </c>
@@ -4430,10 +4468,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8B0AB7-EB07-4BA0-B0D1-595B07C9234C}">
-  <dimension ref="A1:N250"/>
+  <dimension ref="B1:N250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G107" sqref="G107"/>
+    <sheetView tabSelected="1" topLeftCell="B98" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F106" sqref="F106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4446,7 +4484,7 @@
     <col min="6" max="6" width="26.85546875" style="33" customWidth="1"/>
     <col min="7" max="7" width="32.5703125" style="33" customWidth="1"/>
     <col min="8" max="8" width="29" style="33" customWidth="1"/>
-    <col min="9" max="9" width="21.85546875" style="33" customWidth="1"/>
+    <col min="9" max="9" width="45.140625" style="33" customWidth="1"/>
     <col min="10" max="10" width="25.28515625" style="33" customWidth="1"/>
     <col min="11" max="11" width="29" style="33" customWidth="1"/>
     <col min="12" max="12" width="16.7109375" style="33"/>
@@ -4458,7 +4496,7 @@
     <row r="1" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="38" t="s">
         <v>122</v>
       </c>
     </row>
@@ -4475,13 +4513,13 @@
       <c r="E4" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="G4" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="38" t="s">
         <v>136</v>
       </c>
     </row>
@@ -4610,7 +4648,7 @@
         <v>3</v>
       </c>
       <c r="N8" s="34" t="s">
-        <v>334</v>
+        <v>373</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -4750,10 +4788,10 @@
       <c r="E14" s="34">
         <v>3</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="38" t="s">
         <v>134</v>
       </c>
     </row>
@@ -5063,7 +5101,7 @@
     </row>
     <row r="26" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:13" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="38" t="s">
         <v>131</v>
       </c>
       <c r="G27" s="33" t="s">
@@ -5436,7 +5474,7 @@
     </row>
     <row r="42" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="38" t="s">
         <v>139</v>
       </c>
     </row>
@@ -5695,7 +5733,7 @@
     </row>
     <row r="55" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="47" t="s">
+      <c r="B56" s="38" t="s">
         <v>135</v>
       </c>
     </row>
@@ -5707,13 +5745,13 @@
         <v>193</v>
       </c>
       <c r="D57" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="F57" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="G57" s="3" t="s">
         <v>197</v>
@@ -5730,10 +5768,10 @@
         <v>1</v>
       </c>
       <c r="C58" s="34" t="s">
-        <v>335</v>
-      </c>
-      <c r="D58" s="37" t="s">
-        <v>345</v>
+        <v>334</v>
+      </c>
+      <c r="D58" s="35" t="s">
+        <v>344</v>
       </c>
       <c r="E58" s="34" t="s">
         <v>281</v>
@@ -5742,10 +5780,13 @@
         <v>123456789</v>
       </c>
       <c r="G58" s="34" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H58" s="36" t="s">
         <v>301</v>
+      </c>
+      <c r="I58" s="34">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5753,10 +5794,10 @@
         <v>2</v>
       </c>
       <c r="C59" s="34" t="s">
-        <v>336</v>
-      </c>
-      <c r="D59" s="38" t="s">
-        <v>346</v>
+        <v>335</v>
+      </c>
+      <c r="D59" s="34" t="s">
+        <v>345</v>
       </c>
       <c r="E59" s="34" t="s">
         <v>282</v>
@@ -5765,10 +5806,13 @@
         <v>123456789</v>
       </c>
       <c r="G59" s="34" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H59" s="36" t="s">
         <v>301</v>
+      </c>
+      <c r="I59" s="34">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5776,10 +5820,10 @@
         <v>3</v>
       </c>
       <c r="C60" s="34" t="s">
-        <v>338</v>
-      </c>
-      <c r="D60" s="37" t="s">
-        <v>345</v>
+        <v>337</v>
+      </c>
+      <c r="D60" s="35" t="s">
+        <v>365</v>
       </c>
       <c r="E60" s="34" t="s">
         <v>283</v>
@@ -5788,10 +5832,13 @@
         <v>123456789</v>
       </c>
       <c r="G60" s="34" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H60" s="36" t="s">
         <v>301</v>
+      </c>
+      <c r="I60" s="34">
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5799,10 +5846,10 @@
         <v>4</v>
       </c>
       <c r="C61" s="34" t="s">
-        <v>337</v>
-      </c>
-      <c r="D61" s="38" t="s">
-        <v>346</v>
+        <v>336</v>
+      </c>
+      <c r="D61" s="34" t="s">
+        <v>366</v>
       </c>
       <c r="E61" s="34" t="s">
         <v>284</v>
@@ -5811,10 +5858,13 @@
         <v>123456789</v>
       </c>
       <c r="G61" s="34" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H61" s="36" t="s">
         <v>301</v>
+      </c>
+      <c r="I61" s="34">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5822,10 +5872,10 @@
         <v>5</v>
       </c>
       <c r="C62" s="34" t="s">
-        <v>339</v>
-      </c>
-      <c r="D62" s="37" t="s">
-        <v>345</v>
+        <v>338</v>
+      </c>
+      <c r="D62" s="35" t="s">
+        <v>372</v>
       </c>
       <c r="E62" s="34" t="s">
         <v>285</v>
@@ -5834,10 +5884,13 @@
         <v>123456789</v>
       </c>
       <c r="G62" s="34" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H62" s="36" t="s">
         <v>301</v>
+      </c>
+      <c r="I62" s="34">
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5845,10 +5898,10 @@
         <v>6</v>
       </c>
       <c r="C63" s="34" t="s">
-        <v>340</v>
-      </c>
-      <c r="D63" s="38" t="s">
-        <v>346</v>
+        <v>339</v>
+      </c>
+      <c r="D63" s="34" t="s">
+        <v>367</v>
       </c>
       <c r="E63" s="34" t="s">
         <v>286</v>
@@ -5857,10 +5910,13 @@
         <v>123456789</v>
       </c>
       <c r="G63" s="34" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H63" s="36" t="s">
         <v>301</v>
+      </c>
+      <c r="I63" s="34">
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -5868,10 +5924,10 @@
         <v>7</v>
       </c>
       <c r="C64" s="34" t="s">
-        <v>341</v>
-      </c>
-      <c r="D64" s="37" t="s">
-        <v>345</v>
+        <v>340</v>
+      </c>
+      <c r="D64" s="35" t="s">
+        <v>368</v>
       </c>
       <c r="E64" s="34" t="s">
         <v>287</v>
@@ -5880,21 +5936,24 @@
         <v>123456789</v>
       </c>
       <c r="G64" s="34" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H64" s="36" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="65" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I64" s="34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B65" s="34">
         <v>8</v>
       </c>
       <c r="C65" s="34" t="s">
-        <v>342</v>
-      </c>
-      <c r="D65" s="38" t="s">
-        <v>346</v>
+        <v>341</v>
+      </c>
+      <c r="D65" s="34" t="s">
+        <v>369</v>
       </c>
       <c r="E65" s="34" t="s">
         <v>288</v>
@@ -5903,21 +5962,24 @@
         <v>123456789</v>
       </c>
       <c r="G65" s="34" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H65" s="36" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="66" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I65" s="34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="34">
         <v>9</v>
       </c>
       <c r="C66" s="34" t="s">
-        <v>343</v>
-      </c>
-      <c r="D66" s="37" t="s">
-        <v>345</v>
+        <v>342</v>
+      </c>
+      <c r="D66" s="35" t="s">
+        <v>370</v>
       </c>
       <c r="E66" s="34" t="s">
         <v>289</v>
@@ -5926,21 +5988,24 @@
         <v>123456789</v>
       </c>
       <c r="G66" s="34" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H66" s="36" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="67" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I66" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="34">
         <v>10</v>
       </c>
       <c r="C67" s="34" t="s">
-        <v>344</v>
-      </c>
-      <c r="D67" s="38" t="s">
-        <v>346</v>
+        <v>343</v>
+      </c>
+      <c r="D67" s="34" t="s">
+        <v>371</v>
       </c>
       <c r="E67" s="34" t="s">
         <v>290</v>
@@ -5949,28 +6014,31 @@
         <v>123456789</v>
       </c>
       <c r="G67" s="34" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H67" s="36" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="68" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="47" t="s">
+      <c r="I67" s="34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="39" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="71" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B71" s="15" t="s">
         <v>202</v>
       </c>
       <c r="C71" s="32" t="s">
+        <v>356</v>
+      </c>
+      <c r="D71" s="32" t="s">
         <v>357</v>
-      </c>
-      <c r="D71" s="32" t="s">
-        <v>358</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>203</v>
@@ -5979,54 +6047,54 @@
         <v>209</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C73" s="44" t="s">
-        <v>359</v>
-      </c>
-      <c r="D73" s="44"/>
-      <c r="E73" s="44"/>
-    </row>
-    <row r="74" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C74" s="44"/>
-      <c r="D74" s="44"/>
-      <c r="E74" s="44"/>
-    </row>
-    <row r="75" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B76" s="47" t="s">
+    <row r="72" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="45" t="s">
+        <v>358</v>
+      </c>
+      <c r="D73" s="45"/>
+      <c r="E73" s="45"/>
+    </row>
+    <row r="74" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="45"/>
+      <c r="D74" s="45"/>
+      <c r="E74" s="45"/>
+    </row>
+    <row r="75" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="39" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="77" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="15" t="s">
         <v>211</v>
       </c>
       <c r="C77" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="D77" s="15" t="s">
         <v>360</v>
-      </c>
-      <c r="D77" s="15" t="s">
-        <v>361</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="78" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C79" s="44" t="s">
-        <v>359</v>
-      </c>
-      <c r="D79" s="44"/>
-    </row>
-    <row r="80" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C80" s="44"/>
-      <c r="D80" s="44"/>
+    <row r="78" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="45" t="s">
+        <v>358</v>
+      </c>
+      <c r="D79" s="45"/>
+    </row>
+    <row r="80" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="45"/>
+      <c r="D80" s="45"/>
     </row>
     <row r="81" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="82" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="83" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B83" s="16" t="s">
+      <c r="B83" s="38" t="s">
         <v>140</v>
       </c>
     </row>
@@ -6050,36 +6118,40 @@
         <v>148</v>
       </c>
     </row>
-    <row r="85" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="33" t="s">
+        <v>374</v>
+      </c>
+    </row>
     <row r="86" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C86" s="45" t="s">
-        <v>368</v>
-      </c>
-      <c r="D86" s="44"/>
-      <c r="E86" s="44"/>
-      <c r="F86" s="44"/>
+      <c r="C86" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="D86" s="45"/>
+      <c r="E86" s="45"/>
+      <c r="F86" s="45"/>
     </row>
     <row r="87" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C87" s="44"/>
-      <c r="D87" s="44"/>
-      <c r="E87" s="44"/>
-      <c r="F87" s="44"/>
+      <c r="C87" s="45"/>
+      <c r="D87" s="45"/>
+      <c r="E87" s="45"/>
+      <c r="F87" s="45"/>
     </row>
     <row r="88" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C88" s="44"/>
-      <c r="D88" s="44"/>
-      <c r="E88" s="44"/>
-      <c r="F88" s="44"/>
+      <c r="C88" s="45"/>
+      <c r="D88" s="45"/>
+      <c r="E88" s="45"/>
+      <c r="F88" s="45"/>
     </row>
     <row r="89" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C89" s="44"/>
-      <c r="D89" s="44"/>
-      <c r="E89" s="44"/>
-      <c r="F89" s="44"/>
+      <c r="C89" s="45"/>
+      <c r="D89" s="45"/>
+      <c r="E89" s="45"/>
+      <c r="F89" s="45"/>
     </row>
     <row r="90" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="91" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="47" t="s">
+      <c r="B91" s="38" t="s">
         <v>149</v>
       </c>
     </row>
@@ -6092,132 +6164,483 @@
       </c>
     </row>
     <row r="93" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="46" t="s">
-        <v>362</v>
-      </c>
-      <c r="C93" s="46"/>
+      <c r="B93" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="C93" s="47"/>
     </row>
     <row r="94" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="44"/>
-      <c r="C94" s="44"/>
+      <c r="B94" s="45"/>
+      <c r="C94" s="45"/>
     </row>
     <row r="95" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="44"/>
-      <c r="C95" s="44"/>
+      <c r="B95" s="45"/>
+      <c r="C95" s="45"/>
     </row>
     <row r="96" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="48" t="s">
+    <row r="97" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="38" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="98" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B98" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="C98" s="31" t="s">
+      <c r="C98" s="15" t="s">
         <v>170</v>
       </c>
       <c r="D98" s="3" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B99" s="46" t="s">
+      <c r="F98" s="38" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="48" t="s">
+        <v>362</v>
+      </c>
+      <c r="C99" s="48"/>
+      <c r="D99" s="48"/>
+      <c r="F99" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="G99" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="100" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="48"/>
+      <c r="C100" s="48"/>
+      <c r="D100" s="48"/>
+    </row>
+    <row r="101" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B101" s="48"/>
+      <c r="C101" s="48"/>
+      <c r="D101" s="48"/>
+      <c r="F101" s="37" t="s">
+        <v>378</v>
+      </c>
+      <c r="H101" s="33" t="s">
+        <v>334</v>
+      </c>
+      <c r="I101" s="33" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="102" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="33">
+        <v>1</v>
+      </c>
+      <c r="C102" s="33">
+        <v>1</v>
+      </c>
+      <c r="D102" s="33">
+        <v>2</v>
+      </c>
+      <c r="F102" s="37" t="s">
+        <v>379</v>
+      </c>
+      <c r="H102" s="33" t="s">
+        <v>375</v>
+      </c>
+      <c r="I102" s="40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B103" s="33">
+        <v>1</v>
+      </c>
+      <c r="C103" s="33">
+        <v>3</v>
+      </c>
+      <c r="D103" s="33">
+        <v>4</v>
+      </c>
+      <c r="F103" s="37" t="s">
+        <v>380</v>
+      </c>
+      <c r="H103" s="33" t="s">
+        <v>376</v>
+      </c>
+      <c r="I103" s="40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B104" s="33">
+        <v>2</v>
+      </c>
+      <c r="C104" s="33">
+        <v>4</v>
+      </c>
+      <c r="D104" s="33">
+        <v>2</v>
+      </c>
+      <c r="F104" s="37" t="s">
         <v>363</v>
       </c>
-      <c r="C99" s="46"/>
-      <c r="D99" s="46"/>
-    </row>
-    <row r="100" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B100" s="44"/>
-      <c r="C100" s="44"/>
-      <c r="D100" s="44"/>
-    </row>
-    <row r="101" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" s="44"/>
-      <c r="C101" s="44"/>
-      <c r="D101" s="44"/>
-    </row>
-    <row r="102" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="33" t="s">
-        <v>369</v>
-      </c>
-      <c r="B103" s="47" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="C104" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="D104" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B106" s="39" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B107" s="39" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B108" s="39" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B109" s="39" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" spans="1:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="H104" s="33" t="s">
+        <v>377</v>
+      </c>
+      <c r="I104" s="40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B105" s="33">
+        <v>2</v>
+      </c>
+      <c r="C105" s="33">
+        <v>5</v>
+      </c>
+      <c r="D105" s="33">
+        <v>2</v>
+      </c>
+      <c r="F105" s="37" t="s">
+        <v>383</v>
+      </c>
+      <c r="H105" s="33" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B106" s="33">
+        <v>3</v>
+      </c>
+      <c r="C106" s="33">
+        <v>6</v>
+      </c>
+      <c r="D106" s="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B107" s="33">
+        <v>3</v>
+      </c>
+      <c r="C107" s="33">
+        <v>2</v>
+      </c>
+      <c r="D107" s="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B108" s="33">
+        <v>4</v>
+      </c>
+      <c r="C108" s="33">
+        <v>8</v>
+      </c>
+      <c r="D108" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B109" s="33">
+        <v>4</v>
+      </c>
+      <c r="C109" s="33">
+        <v>12</v>
+      </c>
+      <c r="D109" s="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B110" s="33">
+        <v>5</v>
+      </c>
+      <c r="C110" s="33">
+        <v>88</v>
+      </c>
+      <c r="D110" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B111" s="33">
+        <v>5</v>
+      </c>
+      <c r="C111" s="33">
+        <v>22</v>
+      </c>
+      <c r="D111" s="33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="2:9" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B112" s="33">
+        <v>5</v>
+      </c>
+      <c r="C112" s="33">
+        <v>11</v>
+      </c>
+      <c r="D112" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B113" s="33">
+        <v>5</v>
+      </c>
+      <c r="C113" s="33">
+        <v>33</v>
+      </c>
+      <c r="D113" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B114" s="33">
+        <v>6</v>
+      </c>
+      <c r="C114" s="33">
+        <v>2</v>
+      </c>
+      <c r="D114" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B115" s="33">
+        <v>7</v>
+      </c>
+      <c r="C115" s="33">
+        <v>1</v>
+      </c>
+      <c r="D115" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B116" s="33">
+        <v>8</v>
+      </c>
+      <c r="C116" s="33">
+        <v>27</v>
+      </c>
+      <c r="D116" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B117" s="33">
+        <v>8</v>
+      </c>
+      <c r="C117" s="33">
+        <v>23</v>
+      </c>
+      <c r="D117" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B118" s="33">
+        <v>8</v>
+      </c>
+      <c r="C118" s="33">
+        <v>98</v>
+      </c>
+      <c r="D118" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B119" s="33">
+        <v>9</v>
+      </c>
+      <c r="C119" s="33">
+        <v>100</v>
+      </c>
+      <c r="D119" s="33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B120" s="33">
+        <v>9</v>
+      </c>
+      <c r="C120" s="33">
+        <v>11</v>
+      </c>
+      <c r="D120" s="33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B121" s="33">
+        <v>9</v>
+      </c>
+      <c r="C121" s="33">
+        <v>45</v>
+      </c>
+      <c r="D121" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B122" s="33">
+        <v>9</v>
+      </c>
+      <c r="C122" s="33">
+        <v>22</v>
+      </c>
+      <c r="D122" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B123" s="33">
+        <v>9</v>
+      </c>
+      <c r="C123" s="33">
+        <v>32</v>
+      </c>
+      <c r="D123" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B124" s="33">
+        <v>10</v>
+      </c>
+      <c r="C124" s="33">
+        <v>18</v>
+      </c>
+      <c r="D124" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B125" s="33">
+        <v>10</v>
+      </c>
+      <c r="C125" s="33">
+        <v>29</v>
+      </c>
+      <c r="D125" s="33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B126" s="33">
+        <v>11</v>
+      </c>
+      <c r="C126" s="33">
+        <v>33</v>
+      </c>
+      <c r="D126" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B127" s="33">
+        <v>11</v>
+      </c>
+      <c r="C127" s="33">
+        <v>65</v>
+      </c>
+      <c r="D127" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B128" s="33">
+        <v>11</v>
+      </c>
+      <c r="C128" s="33">
+        <v>1</v>
+      </c>
+      <c r="D128" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B129" s="33">
+        <v>11</v>
+      </c>
+      <c r="C129" s="33">
+        <v>2</v>
+      </c>
+      <c r="D129" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B130" s="33">
+        <v>11</v>
+      </c>
+      <c r="C130" s="33">
+        <v>5</v>
+      </c>
+      <c r="D130" s="33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B131" s="33">
+        <v>11</v>
+      </c>
+      <c r="C131" s="33">
+        <v>7</v>
+      </c>
+      <c r="D131" s="33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B132" s="33">
+        <v>12</v>
+      </c>
+      <c r="C132" s="33">
+        <v>55</v>
+      </c>
+      <c r="D132" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B133" s="33">
+        <v>13</v>
+      </c>
+      <c r="C133" s="33">
+        <v>92</v>
+      </c>
+      <c r="D133" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B134" s="33">
+        <v>13</v>
+      </c>
+      <c r="C134" s="33">
+        <v>14</v>
+      </c>
+      <c r="D134" s="33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="2:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="145" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="146" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="147" s="33" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6333,19 +6756,7 @@
     <mergeCell ref="B99:D101"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D58" r:id="rId1" display="nv11@gmal.com" xr:uid="{7DF6E2BD-3B49-4FAA-B3BB-0FCDE51CAA84}"/>
-    <hyperlink ref="D59" r:id="rId2" xr:uid="{E3901EB7-BB24-429D-AE52-F7883B2B5129}"/>
-    <hyperlink ref="D60" r:id="rId3" display="nv11@gmal.com" xr:uid="{261004D4-3860-43B9-8925-2A22E6E33936}"/>
-    <hyperlink ref="D62" r:id="rId4" display="nv11@gmal.com" xr:uid="{928174DC-5C2E-4225-A85A-8278BBE81D33}"/>
-    <hyperlink ref="D64" r:id="rId5" display="nv11@gmal.com" xr:uid="{2460C548-6DC8-4A27-8305-3CFF55F947A1}"/>
-    <hyperlink ref="D66" r:id="rId6" display="nv11@gmal.com" xr:uid="{6284FDF0-BAC9-4683-8471-9663E68E9EB2}"/>
-    <hyperlink ref="D61" r:id="rId7" xr:uid="{260D9451-C344-4B04-B188-3CC2E8B7889A}"/>
-    <hyperlink ref="D63" r:id="rId8" xr:uid="{1BAB657E-613D-4762-9594-DACCCAEDB43A}"/>
-    <hyperlink ref="D65" r:id="rId9" xr:uid="{98F46F85-1924-4E83-B3E9-1256B52B6BE5}"/>
-    <hyperlink ref="D67" r:id="rId10" xr:uid="{F64156F4-4286-43DA-97CE-4FC776A3E52D}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId11"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DML SELECT D2 - 14.05.2024
</commit_message>
<xml_diff>
--- a/java21 database design/Java21 QPhan Database Design.xlsx
+++ b/java21 database design/Java21 QPhan Database Design.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java21\3. Database\java21 database design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD3F05A-3704-4745-AEB0-4247B5A1EDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D65DA2A0-8CEC-4A71-87E2-13B322CF0370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1965" windowWidth="28800" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4470,8 +4470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B8B0AB7-EB07-4BA0-B0D1-595B07C9234C}">
   <dimension ref="B1:N250"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B98" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F106" sqref="F106"/>
+    <sheetView tabSelected="1" topLeftCell="B78" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86:F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>